<commit_message>
completed hhs grant code for sharing
</commit_message>
<xml_diff>
--- a/output/joined_taggs_bystate.xlsx
+++ b/output/joined_taggs_bystate.xlsx
@@ -360,42 +360,42 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>geoid</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>state_or_local</t>
+          <t>state</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>state_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>num_records</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_dollars</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>censuspop2018</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>casecount</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>censuspop2010</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>cases_per_100k</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>num_records</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>total_dollars</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -437,39 +437,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>alabama</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C2">
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>34117522</v>
+      </c>
+      <c r="F2">
+        <v>4887871</v>
+      </c>
+      <c r="G2">
         <v>2881</v>
       </c>
-      <c r="D2">
-        <v>4779736</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="G2">
-        <v>64</v>
-      </c>
       <c r="H2">
-        <v>34117522</v>
+        <v>59</v>
       </c>
       <c r="I2">
-        <v>7.137951133702782</v>
+        <v>6.98003732095221</v>
       </c>
       <c r="J2">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K2">
         <v>11842.24991322457</v>
@@ -478,51 +478,51 @@
         <v>30</v>
       </c>
       <c r="M2">
-        <v>568625.3666666667</v>
+        <v>578263.0847457628</v>
       </c>
       <c r="N2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>alaska</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C3">
+      <c r="D3">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <v>30295475</v>
+      </c>
+      <c r="F3">
+        <v>737438</v>
+      </c>
+      <c r="G3">
         <v>235</v>
       </c>
-      <c r="D3">
-        <v>710231</v>
-      </c>
-      <c r="E3">
-        <v>33</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>AK</t>
-        </is>
-      </c>
-      <c r="G3">
-        <v>110</v>
-      </c>
       <c r="H3">
-        <v>30295475</v>
+        <v>32</v>
       </c>
       <c r="I3">
-        <v>42.65580494233566</v>
+        <v>41.08206384807943</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>128916.914893617</v>
@@ -531,51 +531,51 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>918044.696969697</v>
+        <v>946733.59375</v>
       </c>
       <c r="N3">
         <v>11</v>
       </c>
       <c r="O3">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AZ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>arizona</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C4">
+      <c r="D4">
+        <v>79</v>
+      </c>
+      <c r="E4">
+        <v>49778142</v>
+      </c>
+      <c r="F4">
+        <v>7171646</v>
+      </c>
+      <c r="G4">
         <v>3036</v>
       </c>
-      <c r="D4">
-        <v>6392017</v>
-      </c>
-      <c r="E4">
-        <v>47</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="G4">
-        <v>79</v>
-      </c>
       <c r="H4">
-        <v>49778142</v>
+        <v>42</v>
       </c>
       <c r="I4">
-        <v>7.787548437371178</v>
+        <v>6.940964738081049</v>
       </c>
       <c r="J4">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K4">
         <v>16395.96245059288</v>
@@ -584,51 +584,51 @@
         <v>20</v>
       </c>
       <c r="M4">
-        <v>1059109.404255319</v>
+        <v>1185193.857142857</v>
       </c>
       <c r="N4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O4">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>arkansas</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C5">
+      <c r="D5">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>20471146</v>
+      </c>
+      <c r="F5">
+        <v>3013825</v>
+      </c>
+      <c r="G5">
         <v>1164</v>
       </c>
-      <c r="D5">
-        <v>2915918</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>AR</t>
-        </is>
-      </c>
-      <c r="G5">
-        <v>34</v>
-      </c>
       <c r="H5">
-        <v>20471146</v>
+        <v>39</v>
       </c>
       <c r="I5">
-        <v>7.020480685670859</v>
+        <v>6.792413627201314</v>
       </c>
       <c r="J5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5">
         <v>17586.89518900344</v>
@@ -637,48 +637,48 @@
         <v>17</v>
       </c>
       <c r="M5">
-        <v>511778.65</v>
+        <v>524901.1794871795</v>
       </c>
       <c r="N5">
         <v>27</v>
       </c>
       <c r="O5">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>california</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C6">
+      <c r="D6">
+        <v>564</v>
+      </c>
+      <c r="E6">
+        <v>329575212</v>
+      </c>
+      <c r="F6">
+        <v>39557045</v>
+      </c>
+      <c r="G6">
         <v>20223</v>
       </c>
-      <c r="D6">
-        <v>37253956</v>
-      </c>
-      <c r="E6">
-        <v>54</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G6">
-        <v>564</v>
-      </c>
       <c r="H6">
-        <v>329575212</v>
+        <v>51</v>
       </c>
       <c r="I6">
-        <v>8.846717164748894</v>
+        <v>8.331643882903791</v>
       </c>
       <c r="J6">
         <v>24</v>
@@ -690,51 +690,51 @@
         <v>21</v>
       </c>
       <c r="M6">
-        <v>6103244.666666667</v>
+        <v>6462259.05882353</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>colorado</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C7">
+      <c r="D7">
+        <v>73</v>
+      </c>
+      <c r="E7">
+        <v>46734343</v>
+      </c>
+      <c r="F7">
+        <v>5695564</v>
+      </c>
+      <c r="G7">
         <v>6202</v>
       </c>
-      <c r="D7">
-        <v>5029196</v>
-      </c>
-      <c r="E7">
-        <v>123</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="G7">
-        <v>73</v>
-      </c>
       <c r="H7">
-        <v>46734343</v>
+        <v>109</v>
       </c>
       <c r="I7">
-        <v>9.292607207991098</v>
+        <v>8.205393355249806</v>
       </c>
       <c r="J7">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K7">
         <v>7535.366494679136</v>
@@ -743,51 +743,51 @@
         <v>36</v>
       </c>
       <c r="M7">
-        <v>379954.0081300813</v>
+        <v>428755.4403669725</v>
       </c>
       <c r="N7">
         <v>32</v>
       </c>
       <c r="O7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>connecticut</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C8">
+      <c r="D8">
+        <v>64</v>
+      </c>
+      <c r="E8">
+        <v>33012783</v>
+      </c>
+      <c r="F8">
+        <v>3572665</v>
+      </c>
+      <c r="G8">
         <v>9784</v>
       </c>
-      <c r="D8">
-        <v>3574097</v>
-      </c>
-      <c r="E8">
+      <c r="H8">
         <v>274</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>CT</t>
-        </is>
-      </c>
-      <c r="G8">
-        <v>64</v>
-      </c>
-      <c r="H8">
-        <v>33012783</v>
-      </c>
       <c r="I8">
-        <v>9.236677963692648</v>
+        <v>9.240380220367708</v>
       </c>
       <c r="J8">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K8">
         <v>3374.16015944399</v>
@@ -802,45 +802,45 @@
         <v>46</v>
       </c>
       <c r="O8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>delaware</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C9">
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>8882569</v>
+      </c>
+      <c r="F9">
+        <v>967171</v>
+      </c>
+      <c r="G9">
         <v>1209</v>
       </c>
-      <c r="D9">
-        <v>897934</v>
-      </c>
-      <c r="E9">
-        <v>135</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
       <c r="H9">
-        <v>8882569</v>
+        <v>125</v>
       </c>
       <c r="I9">
-        <v>9.89222927297552</v>
+        <v>9.184072930226403</v>
       </c>
       <c r="J9">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K9">
         <v>7347.038047973532</v>
@@ -849,1388 +849,1388 @@
         <v>37</v>
       </c>
       <c r="M9">
-        <v>65796.80740740741</v>
+        <v>71060.552</v>
       </c>
       <c r="N9">
         <v>51</v>
       </c>
       <c r="O9">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>florida</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>17531</v>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>district of columbia</t>
+        </is>
       </c>
       <c r="D10">
-        <v>18801310</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>93</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>FL</t>
-        </is>
+        <v>25905496</v>
+      </c>
+      <c r="F10">
+        <v>702455</v>
       </c>
       <c r="G10">
-        <v>163</v>
+        <v>1660</v>
       </c>
       <c r="H10">
-        <v>128572709</v>
+        <v>236</v>
       </c>
       <c r="I10">
-        <v>6.838497370661938</v>
+        <v>36.8785132143696</v>
       </c>
       <c r="J10">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>7334.020249843135</v>
+        <v>15605.72048192771</v>
       </c>
       <c r="L10">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="M10">
-        <v>1382502.247311828</v>
+        <v>109769.0508474576</v>
       </c>
       <c r="N10">
+        <v>48</v>
+      </c>
+      <c r="O10">
         <v>6</v>
-      </c>
-      <c r="O10">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>georgia</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>10885</v>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>florida</t>
+        </is>
       </c>
       <c r="D11">
-        <v>9687653</v>
+        <v>163</v>
       </c>
       <c r="E11">
-        <v>112</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
+        <v>128572709</v>
+      </c>
+      <c r="F11">
+        <v>21299325</v>
       </c>
       <c r="G11">
-        <v>98</v>
+        <v>17531</v>
       </c>
       <c r="H11">
-        <v>71962578</v>
+        <v>82</v>
       </c>
       <c r="I11">
-        <v>7.428277829521764</v>
+        <v>6.036468714384141</v>
       </c>
       <c r="J11">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="K11">
-        <v>6611.169315571888</v>
+        <v>7334.020249843135</v>
       </c>
       <c r="L11">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="M11">
-        <v>642523.0178571428</v>
+        <v>1567959.865853659</v>
       </c>
       <c r="N11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O11">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>hawaii</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>442</v>
+          <t>GA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>georgia</t>
+        </is>
       </c>
       <c r="D12">
-        <v>1360301</v>
+        <v>98</v>
       </c>
       <c r="E12">
-        <v>32</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>HI</t>
-        </is>
+        <v>71962578</v>
+      </c>
+      <c r="F12">
+        <v>10519475</v>
       </c>
       <c r="G12">
-        <v>38</v>
+        <v>10885</v>
       </c>
       <c r="H12">
-        <v>19630770</v>
+        <v>103</v>
       </c>
       <c r="I12">
-        <v>14.43119574270695</v>
+        <v>6.840890633800641</v>
       </c>
       <c r="J12">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="K12">
-        <v>44413.50678733032</v>
+        <v>6611.169315571888</v>
       </c>
       <c r="L12">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="M12">
-        <v>613461.5625</v>
+        <v>698665.8058252428</v>
       </c>
       <c r="N12">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O12">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>idaho</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>1354</v>
+          <t>HI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>hawaii</t>
+        </is>
       </c>
       <c r="D13">
-        <v>1567582</v>
+        <v>38</v>
       </c>
       <c r="E13">
-        <v>86</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
+        <v>19630770</v>
+      </c>
+      <c r="F13">
+        <v>1420491</v>
       </c>
       <c r="G13">
-        <v>55</v>
+        <v>442</v>
       </c>
       <c r="H13">
-        <v>19050242</v>
+        <v>31</v>
       </c>
       <c r="I13">
-        <v>12.15262869821164</v>
+        <v>13.819707411029</v>
       </c>
       <c r="J13">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>14069.60265878877</v>
+        <v>44413.50678733032</v>
       </c>
       <c r="L13">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="M13">
-        <v>221514.4418604651</v>
+        <v>633250.6451612903</v>
       </c>
       <c r="N13">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="O13">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>illinois</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>16424</v>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>idaho</t>
+        </is>
       </c>
       <c r="D14">
-        <v>12830632</v>
+        <v>55</v>
       </c>
       <c r="E14">
-        <v>128</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>IL</t>
-        </is>
+        <v>19050242</v>
+      </c>
+      <c r="F14">
+        <v>1754208</v>
       </c>
       <c r="G14">
-        <v>133</v>
+        <v>1354</v>
       </c>
       <c r="H14">
-        <v>102146038</v>
+        <v>77</v>
       </c>
       <c r="I14">
-        <v>7.961107293857387</v>
+        <v>10.85973955198015</v>
       </c>
       <c r="J14">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="K14">
-        <v>6219.315513882124</v>
+        <v>14069.60265878877</v>
       </c>
       <c r="L14">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="M14">
-        <v>798015.921875</v>
+        <v>247405.7402597403</v>
       </c>
       <c r="N14">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="O14">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>indiana</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>6907</v>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>illinois</t>
+        </is>
       </c>
       <c r="D15">
-        <v>6483802</v>
+        <v>133</v>
       </c>
       <c r="E15">
-        <v>107</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
+        <v>102146038</v>
+      </c>
+      <c r="F15">
+        <v>12741080</v>
       </c>
       <c r="G15">
-        <v>78</v>
+        <v>16424</v>
       </c>
       <c r="H15">
-        <v>45762425</v>
+        <v>129</v>
       </c>
       <c r="I15">
-        <v>7.057961517023499</v>
+        <v>8.017062760770672</v>
       </c>
       <c r="J15">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="K15">
-        <v>6625.51397133343</v>
+        <v>6219.315513882124</v>
       </c>
       <c r="L15">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M15">
-        <v>427686.214953271</v>
+        <v>791829.7519379845</v>
       </c>
       <c r="N15">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="O15">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>iowa</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C16">
-        <v>1270</v>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>indiana</t>
+        </is>
       </c>
       <c r="D16">
-        <v>3046355</v>
+        <v>78</v>
       </c>
       <c r="E16">
-        <v>42</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>IA</t>
-        </is>
+        <v>45762425</v>
+      </c>
+      <c r="F16">
+        <v>6691878</v>
       </c>
       <c r="G16">
-        <v>41</v>
+        <v>6907</v>
       </c>
       <c r="H16">
-        <v>22061848</v>
+        <v>103</v>
       </c>
       <c r="I16">
-        <v>7.242047627410463</v>
+        <v>6.838502584775155</v>
       </c>
       <c r="J16">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K16">
-        <v>17371.53385826772</v>
+        <v>6625.51397133343</v>
       </c>
       <c r="L16">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="M16">
-        <v>525282.0952380953</v>
+        <v>444295.3883495146</v>
       </c>
       <c r="N16">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="O16">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>kansas</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C17">
-        <v>1117</v>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>iowa</t>
+        </is>
       </c>
       <c r="D17">
-        <v>2853118</v>
+        <v>41</v>
       </c>
       <c r="E17">
-        <v>39</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>KS</t>
-        </is>
+        <v>22061848</v>
+      </c>
+      <c r="F17">
+        <v>3156145</v>
       </c>
       <c r="G17">
-        <v>51</v>
+        <v>1270</v>
       </c>
       <c r="H17">
-        <v>25194340</v>
+        <v>40</v>
       </c>
       <c r="I17">
-        <v>8.830458466842241</v>
+        <v>6.990124978415124</v>
       </c>
       <c r="J17">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K17">
-        <v>22555.36257833483</v>
+        <v>17371.53385826772</v>
       </c>
       <c r="L17">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M17">
-        <v>646008.717948718</v>
+        <v>551546.2</v>
       </c>
       <c r="N17">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="O17">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>kentucky</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C18">
-        <v>1452</v>
+          <t>KS</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>kansas</t>
+        </is>
       </c>
       <c r="D18">
-        <v>4339367</v>
+        <v>51</v>
       </c>
       <c r="E18">
-        <v>33</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>KY</t>
-        </is>
+        <v>25194340</v>
+      </c>
+      <c r="F18">
+        <v>2911510</v>
       </c>
       <c r="G18">
-        <v>67</v>
+        <v>1117</v>
       </c>
       <c r="H18">
-        <v>34508140</v>
+        <v>38</v>
       </c>
       <c r="I18">
-        <v>7.952344201354713</v>
+        <v>8.653358566517031</v>
       </c>
       <c r="J18">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K18">
-        <v>23765.93663911846</v>
+        <v>22555.36257833483</v>
       </c>
       <c r="L18">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M18">
-        <v>1045701.212121212</v>
+        <v>663008.947368421</v>
       </c>
       <c r="N18">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O18">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>louisiana</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C19">
-        <v>18283</v>
+          <t>KY</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>kentucky</t>
+        </is>
       </c>
       <c r="D19">
-        <v>4533372</v>
+        <v>67</v>
       </c>
       <c r="E19">
-        <v>403</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>LA</t>
-        </is>
+        <v>34508140</v>
+      </c>
+      <c r="F19">
+        <v>4468402</v>
       </c>
       <c r="G19">
-        <v>97</v>
+        <v>1452</v>
       </c>
       <c r="H19">
-        <v>43767117</v>
+        <v>32</v>
       </c>
       <c r="I19">
-        <v>9.654428756342961</v>
+        <v>7.722702657460094</v>
       </c>
       <c r="J19">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="K19">
-        <v>2393.869550948969</v>
+        <v>23765.93663911846</v>
       </c>
       <c r="L19">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="M19">
-        <v>108603.2679900744</v>
+        <v>1078379.375</v>
       </c>
       <c r="N19">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="O19">
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>maine</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C20">
-        <v>560</v>
+          <t>LA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>louisiana</t>
+        </is>
       </c>
       <c r="D20">
-        <v>1328361</v>
+        <v>97</v>
       </c>
       <c r="E20">
-        <v>42</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>ME</t>
-        </is>
+        <v>43767117</v>
+      </c>
+      <c r="F20">
+        <v>4659978</v>
       </c>
       <c r="G20">
+        <v>18283</v>
+      </c>
+      <c r="H20">
+        <v>392</v>
+      </c>
+      <c r="I20">
+        <v>9.392129533658743</v>
+      </c>
+      <c r="J20">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <v>2393.869550948969</v>
+      </c>
+      <c r="L20">
         <v>49</v>
       </c>
-      <c r="H20">
-        <v>20145464</v>
-      </c>
-      <c r="I20">
-        <v>15.16565451710792</v>
-      </c>
-      <c r="J20">
-        <v>8</v>
-      </c>
-      <c r="K20">
-        <v>35974.04285714286</v>
-      </c>
-      <c r="L20">
-        <v>6</v>
-      </c>
       <c r="M20">
-        <v>479653.9047619047</v>
+        <v>111650.8086734694</v>
       </c>
       <c r="N20">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="O20">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>maryland</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C21">
-        <v>6968</v>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>maine</t>
+        </is>
       </c>
       <c r="D21">
-        <v>5773552</v>
+        <v>49</v>
       </c>
       <c r="E21">
-        <v>121</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>MD</t>
-        </is>
+        <v>20145464</v>
+      </c>
+      <c r="F21">
+        <v>1338404</v>
       </c>
       <c r="G21">
-        <v>56</v>
+        <v>560</v>
       </c>
       <c r="H21">
-        <v>39760392</v>
+        <v>42</v>
       </c>
       <c r="I21">
-        <v>6.886643092501808</v>
+        <v>15.05185579242142</v>
       </c>
       <c r="J21">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="K21">
-        <v>5706.141216991963</v>
+        <v>35974.04285714286</v>
       </c>
       <c r="L21">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="M21">
-        <v>328598.2809917355</v>
+        <v>479653.9047619047</v>
       </c>
       <c r="N21">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O21">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>massachusetts</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C22">
-        <v>18941</v>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>maryland</t>
+        </is>
       </c>
       <c r="D22">
-        <v>6547629</v>
+        <v>56</v>
       </c>
       <c r="E22">
-        <v>289</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>MA</t>
-        </is>
+        <v>39760392</v>
+      </c>
+      <c r="F22">
+        <v>6042718</v>
       </c>
       <c r="G22">
-        <v>104</v>
+        <v>6968</v>
       </c>
       <c r="H22">
-        <v>59655700</v>
+        <v>115</v>
       </c>
       <c r="I22">
-        <v>9.111038514857821</v>
+        <v>6.579885409181762</v>
       </c>
       <c r="J22">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="K22">
-        <v>3149.55387783116</v>
+        <v>5706.141216991963</v>
       </c>
       <c r="L22">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M22">
-        <v>206421.107266436</v>
+        <v>345742.5391304348</v>
       </c>
       <c r="N22">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="O22">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>michigan</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C23">
-        <v>21504</v>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>massachusetts</t>
+        </is>
       </c>
       <c r="D23">
-        <v>9883640</v>
+        <v>104</v>
       </c>
       <c r="E23">
-        <v>218</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>MI</t>
-        </is>
+        <v>59655700</v>
+      </c>
+      <c r="F23">
+        <v>6902149</v>
       </c>
       <c r="G23">
-        <v>139</v>
+        <v>18941</v>
       </c>
       <c r="H23">
-        <v>66563270</v>
+        <v>274</v>
       </c>
       <c r="I23">
-        <v>6.734691874653468</v>
+        <v>8.643061747870119</v>
       </c>
       <c r="J23">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="K23">
-        <v>3095.390159970238</v>
+        <v>3149.55387783116</v>
       </c>
       <c r="L23">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M23">
-        <v>305336.1009174312</v>
+        <v>217721.5328467153</v>
       </c>
       <c r="N23">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="O23">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>minnesota</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C24">
-        <v>1242</v>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>michigan</t>
+        </is>
       </c>
       <c r="D24">
-        <v>5303925</v>
+        <v>139</v>
       </c>
       <c r="E24">
-        <v>23</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>MN</t>
-        </is>
+        <v>66563270</v>
+      </c>
+      <c r="F24">
+        <v>9995915</v>
       </c>
       <c r="G24">
-        <v>53</v>
+        <v>21504</v>
       </c>
       <c r="H24">
-        <v>31967817</v>
+        <v>215</v>
       </c>
       <c r="I24">
-        <v>6.027200045249509</v>
+        <v>6.659047220789692</v>
       </c>
       <c r="J24">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K24">
-        <v>25738.98309178744</v>
+        <v>3095.390159970238</v>
       </c>
       <c r="L24">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="M24">
-        <v>1389905.086956522</v>
+        <v>309596.6046511628</v>
       </c>
       <c r="N24">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="O24">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>mississippi</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C25">
-        <v>2469</v>
+          <t>MN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>minnesota</t>
+        </is>
       </c>
       <c r="D25">
-        <v>2967297</v>
+        <v>53</v>
       </c>
       <c r="E25">
-        <v>83</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
+        <v>31967817</v>
+      </c>
+      <c r="F25">
+        <v>5611179</v>
       </c>
       <c r="G25">
-        <v>49</v>
+        <v>1242</v>
       </c>
       <c r="H25">
-        <v>27832636</v>
+        <v>22</v>
       </c>
       <c r="I25">
-        <v>9.379794472882223</v>
+        <v>5.697165782806073</v>
       </c>
       <c r="J25">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="K25">
-        <v>11272.83758606723</v>
+        <v>25738.98309178744</v>
       </c>
       <c r="L25">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="M25">
-        <v>335332.9638554217</v>
+        <v>1453082.590909091</v>
       </c>
       <c r="N25">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="O25">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>missouri</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C26">
-        <v>3624</v>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>mississippi</t>
+        </is>
       </c>
       <c r="D26">
-        <v>5988927</v>
+        <v>49</v>
       </c>
       <c r="E26">
-        <v>61</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>MO</t>
-        </is>
+        <v>27832636</v>
+      </c>
+      <c r="F26">
+        <v>2986530</v>
       </c>
       <c r="G26">
-        <v>80</v>
+        <v>2469</v>
       </c>
       <c r="H26">
-        <v>48834120</v>
+        <v>83</v>
       </c>
       <c r="I26">
-        <v>8.154068333108752</v>
+        <v>9.319389391702076</v>
       </c>
       <c r="J26">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="K26">
-        <v>13475.19867549669</v>
+        <v>11272.83758606723</v>
       </c>
       <c r="L26">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M26">
-        <v>800559.3442622951</v>
+        <v>335332.9638554217</v>
       </c>
       <c r="N26">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="O26">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>montana</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C27">
-        <v>354</v>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>missouri</t>
+        </is>
       </c>
       <c r="D27">
-        <v>989415</v>
+        <v>80</v>
       </c>
       <c r="E27">
-        <v>36</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>MT</t>
-        </is>
+        <v>48834120</v>
+      </c>
+      <c r="F27">
+        <v>6126452</v>
       </c>
       <c r="G27">
-        <v>51</v>
+        <v>3624</v>
       </c>
       <c r="H27">
-        <v>19337900</v>
+        <v>59</v>
       </c>
       <c r="I27">
-        <v>19.54478151230778</v>
+        <v>7.971027929379027</v>
       </c>
       <c r="J27">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="K27">
-        <v>54626.83615819209</v>
+        <v>13475.19867549669</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="M27">
-        <v>537163.8888888889</v>
+        <v>827696.9491525424</v>
       </c>
       <c r="N27">
+        <v>12</v>
+      </c>
+      <c r="O27">
         <v>25</v>
-      </c>
-      <c r="O27">
-        <v>44</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>nebraska</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>577</v>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>montana</t>
+        </is>
       </c>
       <c r="D28">
-        <v>1826341</v>
+        <v>51</v>
       </c>
       <c r="E28">
-        <v>32</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
+        <v>19337900</v>
+      </c>
+      <c r="F28">
+        <v>1062305</v>
       </c>
       <c r="G28">
-        <v>29</v>
+        <v>354</v>
       </c>
       <c r="H28">
-        <v>15660506</v>
+        <v>33</v>
       </c>
       <c r="I28">
-        <v>8.574798463156661</v>
+        <v>18.20371738813241</v>
       </c>
       <c r="J28">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="K28">
-        <v>27141.2582322357</v>
+        <v>54626.83615819209</v>
       </c>
       <c r="L28">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M28">
-        <v>489390.8125</v>
+        <v>585996.9696969697</v>
       </c>
       <c r="N28">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O28">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>nevada</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>2493</v>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>nebraska</t>
+        </is>
       </c>
       <c r="D29">
-        <v>2700551</v>
+        <v>29</v>
       </c>
       <c r="E29">
-        <v>92</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>NV</t>
-        </is>
+        <v>15660506</v>
+      </c>
+      <c r="F29">
+        <v>1929268</v>
       </c>
       <c r="G29">
-        <v>39</v>
+        <v>577</v>
       </c>
       <c r="H29">
-        <v>15951518</v>
+        <v>30</v>
       </c>
       <c r="I29">
-        <v>5.906764212192253</v>
+        <v>8.117330510846601</v>
       </c>
       <c r="J29">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="K29">
-        <v>6398.523064580826</v>
+        <v>27141.2582322357</v>
       </c>
       <c r="L29">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="M29">
-        <v>173386.0652173913</v>
+        <v>522016.8666666666</v>
       </c>
       <c r="N29">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="O29">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>new hampshire</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>819</v>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>nevada</t>
+        </is>
       </c>
       <c r="D30">
-        <v>1316470</v>
+        <v>39</v>
       </c>
       <c r="E30">
-        <v>62</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>NH</t>
-        </is>
+        <v>15951518</v>
+      </c>
+      <c r="F30">
+        <v>3034392</v>
       </c>
       <c r="G30">
-        <v>26</v>
+        <v>2493</v>
       </c>
       <c r="H30">
-        <v>13838597</v>
+        <v>82</v>
       </c>
       <c r="I30">
-        <v>10.51189696688873</v>
+        <v>5.2569074793237</v>
       </c>
       <c r="J30">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="K30">
-        <v>16896.94383394383</v>
+        <v>6398.523064580826</v>
       </c>
       <c r="L30">
+        <v>42</v>
+      </c>
+      <c r="M30">
+        <v>194530.7073170732</v>
+      </c>
+      <c r="N30">
+        <v>43</v>
+      </c>
+      <c r="O30">
         <v>19</v>
-      </c>
-      <c r="M30">
-        <v>223203.1774193548</v>
-      </c>
-      <c r="N30">
-        <v>39</v>
-      </c>
-      <c r="O30">
-        <v>24</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>new jersey</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>54588</v>
+          <t>NH</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>new hampshire</t>
+        </is>
       </c>
       <c r="D31">
-        <v>8791894</v>
+        <v>26</v>
       </c>
       <c r="E31">
-        <v>621</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>NJ</t>
-        </is>
+        <v>13838597</v>
+      </c>
+      <c r="F31">
+        <v>1356458</v>
       </c>
       <c r="G31">
-        <v>76</v>
+        <v>819</v>
       </c>
       <c r="H31">
-        <v>55524423</v>
+        <v>60</v>
       </c>
       <c r="I31">
-        <v>6.315410877337693</v>
+        <v>10.20200920338116</v>
       </c>
       <c r="J31">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="K31">
-        <v>1017.154374587822</v>
+        <v>16896.94383394383</v>
       </c>
       <c r="L31">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="M31">
-        <v>89411.30917874396</v>
+        <v>230643.2833333333</v>
       </c>
       <c r="N31">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O31">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>new mexico</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>989</v>
+          <t>NJ</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>new jersey</t>
+        </is>
       </c>
       <c r="D32">
-        <v>2059179</v>
+        <v>76</v>
       </c>
       <c r="E32">
-        <v>48</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>NM</t>
-        </is>
+        <v>55524423</v>
+      </c>
+      <c r="F32">
+        <v>8908520</v>
       </c>
       <c r="G32">
-        <v>75</v>
+        <v>54588</v>
       </c>
       <c r="H32">
-        <v>31306643</v>
+        <v>613</v>
       </c>
       <c r="I32">
-        <v>15.20345875710659</v>
+        <v>6.232732597558292</v>
       </c>
       <c r="J32">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="K32">
-        <v>31654.84630940344</v>
+        <v>1017.154374587822</v>
       </c>
       <c r="L32">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="M32">
-        <v>652221.7291666666</v>
+        <v>90578.17781402936</v>
       </c>
       <c r="N32">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="O32">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>new york</t>
+          <t>35</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>161807</v>
+          <t>NM</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>new mexico</t>
+        </is>
       </c>
       <c r="D33">
-        <v>19378102</v>
+        <v>75</v>
       </c>
       <c r="E33">
-        <v>835</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
+        <v>31306643</v>
+      </c>
+      <c r="F33">
+        <v>2095428</v>
       </c>
       <c r="G33">
-        <v>196</v>
+        <v>989</v>
       </c>
       <c r="H33">
-        <v>152607845</v>
+        <v>47</v>
       </c>
       <c r="I33">
-        <v>7.875273078859839</v>
+        <v>14.94045273805638</v>
       </c>
       <c r="J33">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="K33">
-        <v>943.1473607445907</v>
+        <v>31654.84630940344</v>
       </c>
       <c r="L33">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="M33">
-        <v>182763.8862275449</v>
+        <v>666098.7872340425</v>
       </c>
       <c r="N33">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="O33">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>north carolina</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>3962</v>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>new york</t>
+        </is>
       </c>
       <c r="D34">
-        <v>9535483</v>
+        <v>196</v>
       </c>
       <c r="E34">
-        <v>42</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>NC</t>
-        </is>
+        <v>152607845</v>
+      </c>
+      <c r="F34">
+        <v>19542209</v>
       </c>
       <c r="G34">
-        <v>136</v>
+        <v>161807</v>
       </c>
       <c r="H34">
-        <v>60229488</v>
+        <v>828</v>
       </c>
       <c r="I34">
-        <v>6.316354189924097</v>
+        <v>7.809139949327121</v>
       </c>
       <c r="J34">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="K34">
-        <v>15201.78899545684</v>
+        <v>943.1473607445907</v>
       </c>
       <c r="L34">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="M34">
-        <v>1434035.428571429</v>
+        <v>184308.9915458937</v>
       </c>
       <c r="N34">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="O34">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>north dakota</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>269</v>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>north carolina</t>
+        </is>
       </c>
       <c r="D35">
-        <v>672591</v>
+        <v>136</v>
       </c>
       <c r="E35">
-        <v>40</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
+        <v>60229488</v>
+      </c>
+      <c r="F35">
+        <v>10383620</v>
       </c>
       <c r="G35">
-        <v>19</v>
+        <v>3962</v>
       </c>
       <c r="H35">
-        <v>9641944</v>
+        <v>38</v>
       </c>
       <c r="I35">
-        <v>14.33552337155864</v>
+        <v>5.800432604428899</v>
       </c>
       <c r="J35">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="K35">
-        <v>35843.65799256506</v>
+        <v>15201.78899545684</v>
       </c>
       <c r="L35">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="M35">
-        <v>241048.6</v>
+        <v>1584986.526315789</v>
       </c>
       <c r="N35">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="O35">
         <v>41</v>
@@ -2239,902 +2239,902 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ohio</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C36">
-        <v>5512</v>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>north dakota</t>
+        </is>
       </c>
       <c r="D36">
-        <v>11536504</v>
+        <v>19</v>
       </c>
       <c r="E36">
-        <v>48</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>OH</t>
-        </is>
+        <v>9641944</v>
+      </c>
+      <c r="F36">
+        <v>760077</v>
       </c>
       <c r="G36">
-        <v>130</v>
+        <v>269</v>
       </c>
       <c r="H36">
-        <v>76966291</v>
+        <v>35</v>
       </c>
       <c r="I36">
-        <v>6.671543736300009</v>
+        <v>12.68548318130926</v>
       </c>
       <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="K36">
+        <v>35843.65799256506</v>
+      </c>
+      <c r="L36">
+        <v>7</v>
+      </c>
+      <c r="M36">
+        <v>275484.1142857143</v>
+      </c>
+      <c r="N36">
+        <v>37</v>
+      </c>
+      <c r="O36">
         <v>43</v>
-      </c>
-      <c r="K36">
-        <v>13963.40547895501</v>
-      </c>
-      <c r="L36">
-        <v>26</v>
-      </c>
-      <c r="M36">
-        <v>1603464.395833333</v>
-      </c>
-      <c r="N36">
-        <v>3</v>
-      </c>
-      <c r="O36">
-        <v>32</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>oklahoma</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C37">
-        <v>1686</v>
+          <t>OH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ohio</t>
+        </is>
       </c>
       <c r="D37">
-        <v>3751351</v>
+        <v>130</v>
       </c>
       <c r="E37">
-        <v>45</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
+        <v>76966291</v>
+      </c>
+      <c r="F37">
+        <v>11689442</v>
       </c>
       <c r="G37">
-        <v>89</v>
+        <v>5512</v>
       </c>
       <c r="H37">
-        <v>35271126</v>
+        <v>47</v>
       </c>
       <c r="I37">
-        <v>9.402246284072058</v>
+        <v>6.584257058634621</v>
       </c>
       <c r="J37">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="K37">
-        <v>20920.00355871886</v>
+        <v>13963.40547895501</v>
       </c>
       <c r="L37">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="M37">
-        <v>783802.8</v>
+        <v>1637580.659574468</v>
       </c>
       <c r="N37">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="O37">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>oregon</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C38">
-        <v>1322</v>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>oklahoma</t>
+        </is>
       </c>
       <c r="D38">
-        <v>3831074</v>
+        <v>89</v>
       </c>
       <c r="E38">
-        <v>35</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
+        <v>35271126</v>
+      </c>
+      <c r="F38">
+        <v>3943079</v>
       </c>
       <c r="G38">
-        <v>116</v>
+        <v>1686</v>
       </c>
       <c r="H38">
-        <v>42445964</v>
+        <v>43</v>
       </c>
       <c r="I38">
-        <v>11.07939027019577</v>
+        <v>8.945072112427876</v>
       </c>
       <c r="J38">
+        <v>20</v>
+      </c>
+      <c r="K38">
+        <v>20920.00355871886</v>
+      </c>
+      <c r="L38">
+        <v>16</v>
+      </c>
+      <c r="M38">
+        <v>820258.7441860465</v>
+      </c>
+      <c r="N38">
         <v>14</v>
       </c>
-      <c r="K38">
-        <v>32107.38577912254</v>
-      </c>
-      <c r="L38">
-        <v>8</v>
-      </c>
-      <c r="M38">
-        <v>1212741.828571429</v>
-      </c>
-      <c r="N38">
-        <v>7</v>
-      </c>
       <c r="O38">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>pennsylvania</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C39">
-        <v>18633</v>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>oregon</t>
+        </is>
       </c>
       <c r="D39">
-        <v>12702379</v>
+        <v>116</v>
       </c>
       <c r="E39">
-        <v>147</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>PA</t>
-        </is>
+        <v>42445964</v>
+      </c>
+      <c r="F39">
+        <v>4190713</v>
       </c>
       <c r="G39">
-        <v>117</v>
+        <v>1322</v>
       </c>
       <c r="H39">
-        <v>82353417</v>
+        <v>32</v>
       </c>
       <c r="I39">
-        <v>6.483306552260801</v>
+        <v>10.12857812023873</v>
       </c>
       <c r="J39">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K39">
-        <v>4419.76155208501</v>
+        <v>32107.38577912254</v>
       </c>
       <c r="L39">
+        <v>8</v>
+      </c>
+      <c r="M39">
+        <v>1326436.375</v>
+      </c>
+      <c r="N39">
+        <v>7</v>
+      </c>
+      <c r="O39">
         <v>45</v>
-      </c>
-      <c r="M39">
-        <v>560227.3265306122</v>
-      </c>
-      <c r="N39">
-        <v>24</v>
-      </c>
-      <c r="O39">
-        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>rhode island</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C40">
-        <v>1727</v>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>pennsylvania</t>
+        </is>
       </c>
       <c r="D40">
-        <v>1052567</v>
+        <v>117</v>
       </c>
       <c r="E40">
-        <v>164</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>RI</t>
-        </is>
+        <v>82353417</v>
+      </c>
+      <c r="F40">
+        <v>12807060</v>
       </c>
       <c r="G40">
-        <v>26</v>
+        <v>18633</v>
       </c>
       <c r="H40">
-        <v>15395742</v>
+        <v>145</v>
       </c>
       <c r="I40">
-        <v>14.62685225738599</v>
+        <v>6.430313983068713</v>
       </c>
       <c r="J40">
+        <v>43</v>
+      </c>
+      <c r="K40">
+        <v>4419.76155208501</v>
+      </c>
+      <c r="L40">
+        <v>45</v>
+      </c>
+      <c r="M40">
+        <v>567954.6</v>
+      </c>
+      <c r="N40">
+        <v>25</v>
+      </c>
+      <c r="O40">
         <v>9</v>
-      </c>
-      <c r="K40">
-        <v>8914.731905037637</v>
-      </c>
-      <c r="L40">
-        <v>35</v>
-      </c>
-      <c r="M40">
-        <v>93876.4756097561</v>
-      </c>
-      <c r="N40">
-        <v>48</v>
-      </c>
-      <c r="O40">
-        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>south carolina</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C41">
-        <v>2793</v>
+          <t>RI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>rhode island</t>
+        </is>
       </c>
       <c r="D41">
-        <v>4625364</v>
+        <v>26</v>
       </c>
       <c r="E41">
-        <v>60</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
+        <v>15395742</v>
+      </c>
+      <c r="F41">
+        <v>1057315</v>
       </c>
       <c r="G41">
-        <v>71</v>
+        <v>1727</v>
       </c>
       <c r="H41">
-        <v>36151921</v>
+        <v>163</v>
       </c>
       <c r="I41">
-        <v>7.816016425950477</v>
+        <v>14.56116862051517</v>
       </c>
       <c r="J41">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="K41">
-        <v>12943.75975653419</v>
+        <v>8914.731905037637</v>
       </c>
       <c r="L41">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M41">
-        <v>602532.0166666667</v>
+        <v>94452.40490797546</v>
       </c>
       <c r="N41">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="O41">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>south dakota</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C42">
-        <v>447</v>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>south carolina</t>
+        </is>
       </c>
       <c r="D42">
-        <v>814180</v>
+        <v>71</v>
       </c>
       <c r="E42">
+        <v>36151921</v>
+      </c>
+      <c r="F42">
+        <v>5084127</v>
+      </c>
+      <c r="G42">
+        <v>2793</v>
+      </c>
+      <c r="H42">
         <v>55</v>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="G42">
-        <v>23</v>
-      </c>
-      <c r="H42">
-        <v>10231886</v>
-      </c>
       <c r="I42">
-        <v>12.56710555405439</v>
+        <v>7.11074310299487</v>
       </c>
       <c r="J42">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="K42">
-        <v>22890.12527964206</v>
+        <v>12943.75975653419</v>
       </c>
       <c r="L42">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="M42">
-        <v>186034.2909090909</v>
+        <v>657307.6545454545</v>
       </c>
       <c r="N42">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="O42">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>tennessee</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C43">
-        <v>4634</v>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>south dakota</t>
+        </is>
       </c>
       <c r="D43">
-        <v>6346105</v>
+        <v>23</v>
       </c>
       <c r="E43">
-        <v>73</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>TN</t>
-        </is>
+        <v>10231886</v>
+      </c>
+      <c r="F43">
+        <v>882235</v>
       </c>
       <c r="G43">
-        <v>91</v>
+        <v>447</v>
       </c>
       <c r="H43">
-        <v>53160247</v>
+        <v>51</v>
       </c>
       <c r="I43">
-        <v>8.376830670151218</v>
+        <v>11.59768769092135</v>
       </c>
       <c r="J43">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="K43">
-        <v>11471.78398791541</v>
+        <v>22890.12527964206</v>
       </c>
       <c r="L43">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="M43">
-        <v>728222.5616438356</v>
+        <v>200625.2156862745</v>
       </c>
       <c r="N43">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="O43">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>texas</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C44">
-        <v>11483</v>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>tennessee</t>
+        </is>
       </c>
       <c r="D44">
-        <v>25145561</v>
+        <v>91</v>
       </c>
       <c r="E44">
-        <v>46</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
+        <v>53160247</v>
+      </c>
+      <c r="F44">
+        <v>6770010</v>
       </c>
       <c r="G44">
-        <v>215</v>
+        <v>4634</v>
       </c>
       <c r="H44">
-        <v>162768263</v>
+        <v>68</v>
       </c>
       <c r="I44">
-        <v>6.473041623529497</v>
+        <v>7.852314398353917</v>
       </c>
       <c r="J44">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="K44">
-        <v>14174.71592789341</v>
+        <v>11471.78398791541</v>
       </c>
       <c r="L44">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M44">
-        <v>3538440.5</v>
+        <v>781768.3382352941</v>
       </c>
       <c r="N44">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="O44">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>utah</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C45">
-        <v>1977</v>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>texas</t>
+        </is>
       </c>
       <c r="D45">
-        <v>2763885</v>
+        <v>215</v>
       </c>
       <c r="E45">
-        <v>72</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>UT</t>
-        </is>
+        <v>162768263</v>
+      </c>
+      <c r="F45">
+        <v>28701845</v>
       </c>
       <c r="G45">
-        <v>37</v>
+        <v>11483</v>
       </c>
       <c r="H45">
-        <v>20897088</v>
+        <v>40</v>
       </c>
       <c r="I45">
-        <v>7.560766095550285</v>
+        <v>5.671003484270785</v>
       </c>
       <c r="J45">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="K45">
-        <v>10570.10015174507</v>
+        <v>14174.71592789341</v>
       </c>
       <c r="L45">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="M45">
-        <v>290237.3333333333</v>
+        <v>4069206.575</v>
       </c>
       <c r="N45">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="O45">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>vermont</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C46">
-        <v>679</v>
+          <t>UT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>utah</t>
+        </is>
       </c>
       <c r="D46">
-        <v>625741</v>
+        <v>37</v>
       </c>
       <c r="E46">
-        <v>109</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>VT</t>
-        </is>
+        <v>20897088</v>
+      </c>
+      <c r="F46">
+        <v>3161105</v>
       </c>
       <c r="G46">
-        <v>31</v>
+        <v>1977</v>
       </c>
       <c r="H46">
-        <v>15697419</v>
+        <v>63</v>
       </c>
       <c r="I46">
-        <v>25.08612828630376</v>
+        <v>6.610690881827716</v>
       </c>
       <c r="J46">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="K46">
-        <v>23118.43740795287</v>
+        <v>10570.10015174507</v>
       </c>
       <c r="L46">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="M46">
-        <v>144013.0183486239</v>
+        <v>331699.8095238095</v>
       </c>
       <c r="N46">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="O46">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>virginia</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C47">
-        <v>4509</v>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>vermont</t>
+        </is>
       </c>
       <c r="D47">
-        <v>8001024</v>
+        <v>31</v>
       </c>
       <c r="E47">
-        <v>56</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>VA</t>
-        </is>
+        <v>15697419</v>
+      </c>
+      <c r="F47">
+        <v>626299</v>
       </c>
       <c r="G47">
-        <v>71</v>
+        <v>679</v>
       </c>
       <c r="H47">
-        <v>43497577</v>
+        <v>108</v>
       </c>
       <c r="I47">
-        <v>5.436501252839636</v>
+        <v>25.06377784412876</v>
       </c>
       <c r="J47">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="K47">
-        <v>9646.83455311599</v>
+        <v>23118.43740795287</v>
       </c>
       <c r="L47">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="M47">
-        <v>776742.4464285715</v>
+        <v>145346.4722222222</v>
       </c>
       <c r="N47">
+        <v>45</v>
+      </c>
+      <c r="O47">
         <v>15</v>
-      </c>
-      <c r="O47">
-        <v>28</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>washington</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C48">
-        <v>9753</v>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>virginia</t>
+        </is>
       </c>
       <c r="D48">
-        <v>6724540</v>
+        <v>71</v>
       </c>
       <c r="E48">
-        <v>145</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>WA</t>
-        </is>
+        <v>43497577</v>
+      </c>
+      <c r="F48">
+        <v>8517685</v>
       </c>
       <c r="G48">
-        <v>122</v>
+        <v>4509</v>
       </c>
       <c r="H48">
-        <v>65424260</v>
+        <v>53</v>
       </c>
       <c r="I48">
-        <v>9.729179988519661</v>
+        <v>5.106736983112196</v>
       </c>
       <c r="J48">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="K48">
-        <v>6708.116476981441</v>
+        <v>9646.83455311599</v>
       </c>
       <c r="L48">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M48">
-        <v>451201.7931034483</v>
+        <v>820709</v>
       </c>
       <c r="N48">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="O48">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>west virginia</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C49">
-        <v>536</v>
+          <t>WA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>washington</t>
+        </is>
       </c>
       <c r="D49">
-        <v>1852994</v>
+        <v>122</v>
       </c>
       <c r="E49">
+        <v>65424260</v>
+      </c>
+      <c r="F49">
+        <v>7535591</v>
+      </c>
+      <c r="G49">
+        <v>9753</v>
+      </c>
+      <c r="H49">
+        <v>129</v>
+      </c>
+      <c r="I49">
+        <v>8.682034362002927</v>
+      </c>
+      <c r="J49">
+        <v>21</v>
+      </c>
+      <c r="K49">
+        <v>6708.116476981441</v>
+      </c>
+      <c r="L49">
+        <v>39</v>
+      </c>
+      <c r="M49">
+        <v>507164.8062015504</v>
+      </c>
+      <c r="N49">
         <v>29</v>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>WV</t>
-        </is>
-      </c>
-      <c r="G49">
-        <v>67</v>
-      </c>
-      <c r="H49">
-        <v>30983620</v>
-      </c>
-      <c r="I49">
-        <v>16.72084205345511</v>
-      </c>
-      <c r="J49">
-        <v>6</v>
-      </c>
-      <c r="K49">
-        <v>57805.26119402985</v>
-      </c>
-      <c r="L49">
-        <v>2</v>
-      </c>
-      <c r="M49">
-        <v>1068400.689655172</v>
-      </c>
-      <c r="N49">
-        <v>8</v>
-      </c>
       <c r="O49">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>wisconsin</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C50">
-        <v>2890</v>
+          <t>WV</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>west virginia</t>
+        </is>
       </c>
       <c r="D50">
-        <v>5686986</v>
+        <v>67</v>
       </c>
       <c r="E50">
-        <v>51</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>WI</t>
-        </is>
+        <v>30983620</v>
+      </c>
+      <c r="F50">
+        <v>1805832</v>
       </c>
       <c r="G50">
-        <v>57</v>
+        <v>536</v>
       </c>
       <c r="H50">
-        <v>35249718</v>
+        <v>30</v>
       </c>
       <c r="I50">
-        <v>6.198312779387886</v>
+        <v>17.15753181912825</v>
       </c>
       <c r="J50">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="K50">
-        <v>12197.13425605536</v>
+        <v>57805.26119402985</v>
       </c>
       <c r="L50">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="M50">
-        <v>691170.9411764706</v>
+        <v>1032787.333333333</v>
       </c>
       <c r="N50">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="O50">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>wyoming</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C51">
-        <v>239</v>
+          <t>WI</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>wisconsin</t>
+        </is>
       </c>
       <c r="D51">
-        <v>563626</v>
+        <v>57</v>
       </c>
       <c r="E51">
-        <v>42</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>WY</t>
-        </is>
+        <v>35249718</v>
+      </c>
+      <c r="F51">
+        <v>5813568</v>
       </c>
       <c r="G51">
-        <v>19</v>
+        <v>2890</v>
       </c>
       <c r="H51">
-        <v>10194407</v>
+        <v>50</v>
       </c>
       <c r="I51">
-        <v>18.08718369982932</v>
+        <v>6.063353520591829</v>
       </c>
       <c r="J51">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="K51">
-        <v>42654.42259414226</v>
+        <v>12197.13425605536</v>
       </c>
       <c r="L51">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="M51">
-        <v>242723.9761904762</v>
+        <v>704994.36</v>
       </c>
       <c r="N51">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="O51">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>district of columbia</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>state</t>
-        </is>
-      </c>
-      <c r="C52">
-        <v>1660</v>
+          <t>WY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>wyoming</t>
+        </is>
       </c>
       <c r="D52">
-        <v>601723</v>
+        <v>19</v>
       </c>
       <c r="E52">
-        <v>276</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
+        <v>10194407</v>
+      </c>
+      <c r="F52">
+        <v>577737</v>
       </c>
       <c r="G52">
-        <v>22</v>
+        <v>239</v>
       </c>
       <c r="H52">
-        <v>25905496</v>
+        <v>41</v>
       </c>
       <c r="I52">
-        <v>43.05219511303374</v>
+        <v>17.64541132037588</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K52">
-        <v>15605.72048192771</v>
+        <v>42654.42259414226</v>
       </c>
       <c r="L52">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="M52">
-        <v>93860.49275362318</v>
+        <v>248644.0731707317</v>
       </c>
       <c r="N52">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="O52">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comprehensive update for final code and outputs
</commit_message>
<xml_diff>
--- a/output/joined_taggs_bystate.xlsx
+++ b/output/joined_taggs_bystate.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,22 +365,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>state_name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>state_name</t>
+          <t>total_dollars</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>num_records</t>
+          <t>casecount</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>total_dollars</t>
+          <t>dollars_percase</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -390,47 +390,37 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>casecount</t>
+          <t>dollars_percapita</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cases_per_100k</t>
+          <t>casecount_rank</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>dollars_percapita</t>
+          <t>dollars_percase_rank</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>rankspread_casecount_dollarspercase</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>pop_rank</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>dollars_percapita_rank</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>dollars_percase</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>dollars_percase_rank</t>
-        </is>
-      </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>dollars_per_casesper100kppl</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>dollars_per_casesper100kppl_rank</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>cases_per_100k_rank</t>
+          <t>rankspread_population_dollarsperpop</t>
         </is>
       </c>
     </row>
@@ -442,49 +432,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>alabama</t>
         </is>
       </c>
+      <c r="C2">
+        <v>34117522</v>
+      </c>
       <c r="D2">
-        <v>64</v>
+        <v>3611</v>
       </c>
       <c r="E2">
-        <v>34117522</v>
+        <v>9448.219883688729</v>
       </c>
       <c r="F2">
         <v>4887871</v>
       </c>
       <c r="G2">
-        <v>2881</v>
+        <v>6.98003732095221</v>
       </c>
       <c r="H2">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I2">
-        <v>6.98003732095221</v>
+        <v>31</v>
       </c>
       <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>24</v>
+      </c>
+      <c r="L2">
         <v>34</v>
       </c>
-      <c r="K2">
-        <v>11842.24991322457</v>
-      </c>
-      <c r="L2">
-        <v>30</v>
-      </c>
       <c r="M2">
-        <v>578263.0847457628</v>
-      </c>
-      <c r="N2">
-        <v>24</v>
-      </c>
-      <c r="O2">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -495,49 +477,41 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AK</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>alaska</t>
         </is>
       </c>
+      <c r="C3">
+        <v>30295475</v>
+      </c>
       <c r="D3">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="E3">
-        <v>30295475</v>
+        <v>111380.4227941177</v>
       </c>
       <c r="F3">
         <v>737438</v>
       </c>
       <c r="G3">
-        <v>235</v>
+        <v>41.08206384807943</v>
       </c>
       <c r="H3">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I3">
-        <v>41.08206384807943</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="K3">
-        <v>128916.914893617</v>
+        <v>48</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
       <c r="M3">
-        <v>946733.59375</v>
-      </c>
-      <c r="N3">
-        <v>11</v>
-      </c>
-      <c r="O3">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -548,49 +522,41 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>arizona</t>
         </is>
       </c>
+      <c r="C4">
+        <v>49778142</v>
+      </c>
       <c r="D4">
-        <v>79</v>
+        <v>3542</v>
       </c>
       <c r="E4">
-        <v>49778142</v>
+        <v>14053.68210050819</v>
       </c>
       <c r="F4">
         <v>7171646</v>
       </c>
       <c r="G4">
-        <v>3036</v>
+        <v>6.940964738081049</v>
       </c>
       <c r="H4">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="I4">
-        <v>6.940964738081049</v>
+        <v>18</v>
       </c>
       <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
         <v>35</v>
       </c>
-      <c r="K4">
-        <v>16395.96245059288</v>
-      </c>
-      <c r="L4">
-        <v>20</v>
-      </c>
       <c r="M4">
-        <v>1185193.857142857</v>
-      </c>
-      <c r="N4">
-        <v>8</v>
-      </c>
-      <c r="O4">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -601,49 +567,41 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AR</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>arkansas</t>
         </is>
       </c>
+      <c r="C5">
+        <v>20471146</v>
+      </c>
       <c r="D5">
-        <v>34</v>
+        <v>1398</v>
       </c>
       <c r="E5">
-        <v>20471146</v>
+        <v>14643.16595135908</v>
       </c>
       <c r="F5">
         <v>3013825</v>
       </c>
       <c r="G5">
-        <v>1164</v>
+        <v>6.792413627201314</v>
       </c>
       <c r="H5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5">
-        <v>6.792413627201314</v>
+        <v>16</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="K5">
-        <v>17586.89518900344</v>
+        <v>33</v>
       </c>
       <c r="L5">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="M5">
-        <v>524901.1794871795</v>
-      </c>
-      <c r="N5">
-        <v>27</v>
-      </c>
-      <c r="O5">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +612,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>california</t>
         </is>
       </c>
+      <c r="C6">
+        <v>329575212</v>
+      </c>
       <c r="D6">
-        <v>567</v>
+        <v>23324</v>
       </c>
       <c r="E6">
-        <v>330095107</v>
+        <v>14130.30406448294</v>
       </c>
       <c r="F6">
         <v>39557045</v>
       </c>
       <c r="G6">
-        <v>20223</v>
+        <v>8.331643882903791</v>
       </c>
       <c r="H6">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>8.344786800935207</v>
+        <v>17</v>
       </c>
       <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>24</v>
       </c>
-      <c r="K6">
-        <v>16322.75661375661</v>
-      </c>
-      <c r="L6">
-        <v>21</v>
-      </c>
       <c r="M6">
-        <v>6472453.078431373</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -707,49 +657,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>colorado</t>
         </is>
       </c>
+      <c r="C7">
+        <v>46734343</v>
+      </c>
       <c r="D7">
-        <v>73</v>
+        <v>7307</v>
       </c>
       <c r="E7">
-        <v>46734343</v>
+        <v>6395.83180511838</v>
       </c>
       <c r="F7">
         <v>5695564</v>
       </c>
       <c r="G7">
-        <v>6202</v>
+        <v>8.205393355249806</v>
       </c>
       <c r="H7">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="I7">
-        <v>8.205393355249806</v>
+        <v>36</v>
       </c>
       <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>21</v>
+      </c>
+      <c r="L7">
         <v>25</v>
       </c>
-      <c r="K7">
-        <v>7535.366494679136</v>
-      </c>
-      <c r="L7">
-        <v>36</v>
-      </c>
       <c r="M7">
-        <v>428755.4403669725</v>
-      </c>
-      <c r="N7">
-        <v>32</v>
-      </c>
-      <c r="O7">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -760,49 +702,41 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CT</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>connecticut</t>
         </is>
       </c>
+      <c r="C8">
+        <v>33012783</v>
+      </c>
       <c r="D8">
-        <v>64</v>
+        <v>12035</v>
       </c>
       <c r="E8">
-        <v>33012783</v>
+        <v>2743.064644786041</v>
       </c>
       <c r="F8">
         <v>3572665</v>
       </c>
       <c r="G8">
-        <v>9784</v>
+        <v>9.240380220367708</v>
       </c>
       <c r="H8">
-        <v>274</v>
+        <v>12</v>
       </c>
       <c r="I8">
-        <v>9.240380220367708</v>
+        <v>47</v>
       </c>
       <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="K8">
+        <v>29</v>
+      </c>
+      <c r="L8">
         <v>18</v>
       </c>
-      <c r="K8">
-        <v>3374.16015944399</v>
-      </c>
-      <c r="L8">
-        <v>46</v>
-      </c>
       <c r="M8">
-        <v>120484.6094890511</v>
-      </c>
-      <c r="N8">
-        <v>46</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -813,49 +747,41 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>delaware</t>
         </is>
       </c>
+      <c r="C9">
+        <v>8882569</v>
+      </c>
       <c r="D9">
-        <v>18</v>
+        <v>1625</v>
       </c>
       <c r="E9">
-        <v>8882569</v>
+        <v>5466.196307692308</v>
       </c>
       <c r="F9">
         <v>967171</v>
       </c>
       <c r="G9">
-        <v>1209</v>
+        <v>9.184072930226403</v>
       </c>
       <c r="H9">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="I9">
-        <v>9.184072930226403</v>
+        <v>41</v>
       </c>
       <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
         <v>19</v>
       </c>
-      <c r="K9">
-        <v>7347.038047973532</v>
-      </c>
-      <c r="L9">
-        <v>37</v>
-      </c>
       <c r="M9">
-        <v>71060.552</v>
-      </c>
-      <c r="N9">
-        <v>51</v>
-      </c>
-      <c r="O9">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -866,49 +792,41 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>district of columbia</t>
         </is>
       </c>
+      <c r="C10">
+        <v>15905496</v>
+      </c>
       <c r="D10">
-        <v>22</v>
+        <v>1875</v>
       </c>
       <c r="E10">
-        <v>25905496</v>
+        <v>8482.931200000001</v>
       </c>
       <c r="F10">
         <v>702455</v>
       </c>
       <c r="G10">
-        <v>1660</v>
+        <v>22.64272586856098</v>
       </c>
       <c r="H10">
-        <v>236</v>
+        <v>32</v>
       </c>
       <c r="I10">
-        <v>36.87851321436961</v>
+        <v>33</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>15605.72048192771</v>
+        <v>49</v>
       </c>
       <c r="L10">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="M10">
-        <v>109769.0508474576</v>
-      </c>
-      <c r="N10">
-        <v>48</v>
-      </c>
-      <c r="O10">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
@@ -919,49 +837,41 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>FL</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>florida</t>
         </is>
       </c>
+      <c r="C11">
+        <v>128572709</v>
+      </c>
       <c r="D11">
-        <v>163</v>
+        <v>19895</v>
       </c>
       <c r="E11">
-        <v>128572709</v>
+        <v>6462.563910530284</v>
       </c>
       <c r="F11">
         <v>21299325</v>
       </c>
       <c r="G11">
-        <v>17531</v>
+        <v>6.036468714384141</v>
       </c>
       <c r="H11">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="I11">
-        <v>6.036468714384141</v>
+        <v>35</v>
       </c>
       <c r="J11">
+        <v>26</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
         <v>46</v>
       </c>
-      <c r="K11">
-        <v>7334.020249843135</v>
-      </c>
-      <c r="L11">
-        <v>38</v>
-      </c>
       <c r="M11">
-        <v>1567959.865853659</v>
-      </c>
-      <c r="N11">
-        <v>5</v>
-      </c>
-      <c r="O11">
-        <v>19</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
@@ -972,49 +882,41 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>georgia</t>
         </is>
       </c>
+      <c r="C12">
+        <v>66962578</v>
+      </c>
       <c r="D12">
-        <v>98</v>
+        <v>12550</v>
       </c>
       <c r="E12">
-        <v>71962578</v>
+        <v>5335.66358565737</v>
       </c>
       <c r="F12">
         <v>10519475</v>
       </c>
       <c r="G12">
-        <v>10885</v>
+        <v>6.365581742434865</v>
       </c>
       <c r="H12">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="I12">
-        <v>6.840890633800641</v>
+        <v>42</v>
       </c>
       <c r="J12">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K12">
-        <v>6611.169315571888</v>
+        <v>8</v>
       </c>
       <c r="L12">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M12">
-        <v>698665.8058252428</v>
-      </c>
-      <c r="N12">
-        <v>18</v>
-      </c>
-      <c r="O12">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -1025,49 +927,41 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>HI</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>hawaii</t>
         </is>
       </c>
+      <c r="C13">
+        <v>19630770</v>
+      </c>
       <c r="D13">
-        <v>38</v>
+        <v>499</v>
       </c>
       <c r="E13">
-        <v>19630770</v>
+        <v>39340.22044088176</v>
       </c>
       <c r="F13">
         <v>1420491</v>
       </c>
       <c r="G13">
-        <v>442</v>
+        <v>13.819707411029</v>
       </c>
       <c r="H13">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="I13">
-        <v>13.819707411029</v>
+        <v>4</v>
       </c>
       <c r="J13">
+        <v>43</v>
+      </c>
+      <c r="K13">
+        <v>40</v>
+      </c>
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="K13">
-        <v>44413.50678733032</v>
-      </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
       <c r="M13">
-        <v>633250.6451612903</v>
-      </c>
-      <c r="N13">
-        <v>22</v>
-      </c>
-      <c r="O13">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -1078,49 +972,41 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>idaho</t>
         </is>
       </c>
+      <c r="C14">
+        <v>19050242</v>
+      </c>
       <c r="D14">
-        <v>55</v>
+        <v>1426</v>
       </c>
       <c r="E14">
-        <v>19050242</v>
+        <v>13359.2159887798</v>
       </c>
       <c r="F14">
         <v>1754208</v>
       </c>
       <c r="G14">
-        <v>1354</v>
+        <v>10.85973955198015</v>
       </c>
       <c r="H14">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="I14">
-        <v>10.85973955198015</v>
+        <v>22</v>
       </c>
       <c r="J14">
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <v>39</v>
+      </c>
+      <c r="L14">
         <v>13</v>
       </c>
-      <c r="K14">
-        <v>14069.60265878877</v>
-      </c>
-      <c r="L14">
-        <v>25</v>
-      </c>
       <c r="M14">
-        <v>247405.7402597403</v>
-      </c>
-      <c r="N14">
-        <v>39</v>
-      </c>
-      <c r="O14">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
@@ -1131,49 +1017,41 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>illinois</t>
         </is>
       </c>
+      <c r="C15">
+        <v>102146038</v>
+      </c>
       <c r="D15">
-        <v>133</v>
+        <v>20852</v>
       </c>
       <c r="E15">
-        <v>102146038</v>
+        <v>4898.620659888739</v>
       </c>
       <c r="F15">
         <v>12741080</v>
       </c>
       <c r="G15">
-        <v>16424</v>
+        <v>8.017062760770672</v>
       </c>
       <c r="H15">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="I15">
-        <v>8.017062760770672</v>
+        <v>43</v>
       </c>
       <c r="J15">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K15">
-        <v>6219.315513882124</v>
+        <v>6</v>
       </c>
       <c r="L15">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="M15">
-        <v>791829.7519379845</v>
-      </c>
-      <c r="N15">
-        <v>15</v>
-      </c>
-      <c r="O15">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -1184,49 +1062,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>indiana</t>
         </is>
       </c>
+      <c r="C16">
+        <v>45762425</v>
+      </c>
       <c r="D16">
-        <v>78</v>
+        <v>7928</v>
       </c>
       <c r="E16">
-        <v>45762425</v>
+        <v>5772.253405650858</v>
       </c>
       <c r="F16">
         <v>6691878</v>
       </c>
       <c r="G16">
-        <v>6907</v>
+        <v>6.838502584775156</v>
       </c>
       <c r="H16">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="I16">
-        <v>6.838502584775156</v>
+        <v>39</v>
       </c>
       <c r="J16">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="K16">
-        <v>6625.51397133343</v>
+        <v>17</v>
       </c>
       <c r="L16">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M16">
-        <v>444295.3883495146</v>
-      </c>
-      <c r="N16">
-        <v>31</v>
-      </c>
-      <c r="O16">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -1237,49 +1107,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>IA</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>iowa</t>
         </is>
       </c>
+      <c r="C17">
+        <v>22061848</v>
+      </c>
       <c r="D17">
-        <v>41</v>
+        <v>1587</v>
       </c>
       <c r="E17">
-        <v>22061848</v>
+        <v>13901.60554505356</v>
       </c>
       <c r="F17">
         <v>3156145</v>
       </c>
       <c r="G17">
-        <v>1270</v>
+        <v>6.990124978415124</v>
       </c>
       <c r="H17">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I17">
-        <v>6.990124978415124</v>
+        <v>21</v>
       </c>
       <c r="J17">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>31</v>
+      </c>
+      <c r="L17">
         <v>33</v>
       </c>
-      <c r="K17">
-        <v>17371.53385826772</v>
-      </c>
-      <c r="L17">
-        <v>18</v>
-      </c>
       <c r="M17">
-        <v>551546.2</v>
-      </c>
-      <c r="N17">
-        <v>26</v>
-      </c>
-      <c r="O17">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1290,49 +1152,41 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>KS</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>kansas</t>
         </is>
       </c>
+      <c r="C18">
+        <v>25194340</v>
+      </c>
       <c r="D18">
-        <v>51</v>
+        <v>1344</v>
       </c>
       <c r="E18">
-        <v>25194340</v>
+        <v>18745.78869047619</v>
       </c>
       <c r="F18">
         <v>2911510</v>
       </c>
       <c r="G18">
-        <v>1117</v>
+        <v>8.653358566517031</v>
       </c>
       <c r="H18">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I18">
-        <v>8.653358566517031</v>
+        <v>13</v>
       </c>
       <c r="J18">
+        <v>26</v>
+      </c>
+      <c r="K18">
+        <v>35</v>
+      </c>
+      <c r="L18">
         <v>22</v>
       </c>
-      <c r="K18">
-        <v>22555.36257833483</v>
-      </c>
-      <c r="L18">
-        <v>15</v>
-      </c>
       <c r="M18">
-        <v>663008.947368421</v>
-      </c>
-      <c r="N18">
-        <v>20</v>
-      </c>
-      <c r="O18">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -1343,49 +1197,41 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KY</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>kentucky</t>
         </is>
       </c>
+      <c r="C19">
+        <v>34508140</v>
+      </c>
       <c r="D19">
-        <v>67</v>
+        <v>2018</v>
       </c>
       <c r="E19">
-        <v>34508140</v>
+        <v>17100.16848364718</v>
       </c>
       <c r="F19">
         <v>4468402</v>
       </c>
       <c r="G19">
-        <v>1452</v>
+        <v>7.722702657460094</v>
       </c>
       <c r="H19">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I19">
-        <v>7.722702657460094</v>
+        <v>15</v>
       </c>
       <c r="J19">
+        <v>15</v>
+      </c>
+      <c r="K19">
+        <v>26</v>
+      </c>
+      <c r="L19">
         <v>31</v>
       </c>
-      <c r="K19">
-        <v>23765.93663911846</v>
-      </c>
-      <c r="L19">
-        <v>12</v>
-      </c>
       <c r="M19">
-        <v>1078379.375</v>
-      </c>
-      <c r="N19">
-        <v>9</v>
-      </c>
-      <c r="O19">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -1396,49 +1242,41 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>louisiana</t>
         </is>
       </c>
+      <c r="C20">
+        <v>43767117</v>
+      </c>
       <c r="D20">
-        <v>97</v>
+        <v>20595</v>
       </c>
       <c r="E20">
-        <v>43767117</v>
+        <v>2125.133139111435</v>
       </c>
       <c r="F20">
         <v>4659978</v>
       </c>
       <c r="G20">
-        <v>18283</v>
+        <v>9.392129533658743</v>
       </c>
       <c r="H20">
-        <v>392</v>
+        <v>8</v>
       </c>
       <c r="I20">
-        <v>9.392129533658743</v>
+        <v>49</v>
       </c>
       <c r="J20">
+        <v>41</v>
+      </c>
+      <c r="K20">
+        <v>25</v>
+      </c>
+      <c r="L20">
         <v>16</v>
       </c>
-      <c r="K20">
-        <v>2393.869550948969</v>
-      </c>
-      <c r="L20">
-        <v>49</v>
-      </c>
       <c r="M20">
-        <v>111650.8086734694</v>
-      </c>
-      <c r="N20">
-        <v>47</v>
-      </c>
-      <c r="O20">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -1449,48 +1287,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ME</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
           <t>maine</t>
         </is>
       </c>
+      <c r="C21">
+        <v>20145464</v>
+      </c>
       <c r="D21">
-        <v>49</v>
+        <v>633</v>
       </c>
       <c r="E21">
-        <v>20145464</v>
+        <v>31825.3775671406</v>
       </c>
       <c r="F21">
         <v>1338404</v>
       </c>
       <c r="G21">
-        <v>560</v>
+        <v>15.05185579242142</v>
       </c>
       <c r="H21">
+        <v>45</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>39</v>
+      </c>
+      <c r="K21">
         <v>42</v>
       </c>
-      <c r="I21">
-        <v>15.05185579242142</v>
-      </c>
-      <c r="J21">
+      <c r="L21">
         <v>7</v>
       </c>
-      <c r="K21">
-        <v>35974.04285714286</v>
-      </c>
-      <c r="L21">
-        <v>6</v>
-      </c>
       <c r="M21">
-        <v>479653.9047619047</v>
-      </c>
-      <c r="N21">
-        <v>30</v>
-      </c>
-      <c r="O21">
         <v>35</v>
       </c>
     </row>
@@ -1502,49 +1332,41 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MD</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
           <t>maryland</t>
         </is>
       </c>
+      <c r="C22">
+        <v>39760392</v>
+      </c>
       <c r="D22">
-        <v>58</v>
+        <v>8936</v>
       </c>
       <c r="E22">
-        <v>40319230</v>
+        <v>4449.461951656222</v>
       </c>
       <c r="F22">
         <v>6042718</v>
       </c>
       <c r="G22">
-        <v>6968</v>
+        <v>6.579885409181762</v>
       </c>
       <c r="H22">
-        <v>115</v>
+        <v>14</v>
       </c>
       <c r="I22">
-        <v>6.672366640309874</v>
+        <v>44</v>
       </c>
       <c r="J22">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K22">
-        <v>5786.341848450057</v>
+        <v>19</v>
       </c>
       <c r="L22">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M22">
-        <v>350602</v>
-      </c>
-      <c r="N22">
-        <v>33</v>
-      </c>
-      <c r="O22">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -1555,49 +1377,41 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MA</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
           <t>massachusetts</t>
         </is>
       </c>
+      <c r="C23">
+        <v>59655700</v>
+      </c>
       <c r="D23">
-        <v>104</v>
+        <v>25475</v>
       </c>
       <c r="E23">
-        <v>59655700</v>
+        <v>2341.7350343474</v>
       </c>
       <c r="F23">
         <v>6902149</v>
       </c>
       <c r="G23">
-        <v>18941</v>
+        <v>8.643061747870119</v>
       </c>
       <c r="H23">
-        <v>274</v>
+        <v>3</v>
       </c>
       <c r="I23">
-        <v>8.643061747870119</v>
+        <v>48</v>
       </c>
       <c r="J23">
+        <v>45</v>
+      </c>
+      <c r="K23">
+        <v>15</v>
+      </c>
+      <c r="L23">
         <v>23</v>
       </c>
-      <c r="K23">
-        <v>3149.55387783116</v>
-      </c>
-      <c r="L23">
-        <v>47</v>
-      </c>
       <c r="M23">
-        <v>217721.5328467153</v>
-      </c>
-      <c r="N23">
-        <v>41</v>
-      </c>
-      <c r="O23">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -1608,49 +1422,41 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MI</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
           <t>michigan</t>
         </is>
       </c>
+      <c r="C24">
+        <v>66563270</v>
+      </c>
       <c r="D24">
-        <v>139</v>
+        <v>24244</v>
       </c>
       <c r="E24">
-        <v>66563270</v>
+        <v>2745.556426332289</v>
       </c>
       <c r="F24">
         <v>9995915</v>
       </c>
       <c r="G24">
-        <v>21504</v>
+        <v>6.659047220789693</v>
       </c>
       <c r="H24">
-        <v>215</v>
+        <v>4</v>
       </c>
       <c r="I24">
-        <v>6.659047220789693</v>
+        <v>46</v>
       </c>
       <c r="J24">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K24">
-        <v>3095.390159970238</v>
+        <v>10</v>
       </c>
       <c r="L24">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="M24">
-        <v>309596.6046511628</v>
-      </c>
-      <c r="N24">
-        <v>36</v>
-      </c>
-      <c r="O24">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25">
@@ -1661,49 +1467,41 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>MN</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
           <t>minnesota</t>
         </is>
       </c>
+      <c r="C25">
+        <v>31967817</v>
+      </c>
       <c r="D25">
-        <v>53</v>
+        <v>1621</v>
       </c>
       <c r="E25">
-        <v>31967817</v>
+        <v>19721.04688463911</v>
       </c>
       <c r="F25">
         <v>5611179</v>
       </c>
       <c r="G25">
-        <v>1242</v>
+        <v>5.697165782806073</v>
       </c>
       <c r="H25">
+        <v>34</v>
+      </c>
+      <c r="I25">
+        <v>11</v>
+      </c>
+      <c r="J25">
+        <v>23</v>
+      </c>
+      <c r="K25">
         <v>22</v>
       </c>
-      <c r="I25">
-        <v>5.697165782806073</v>
-      </c>
-      <c r="J25">
+      <c r="L25">
         <v>48</v>
       </c>
-      <c r="K25">
-        <v>25738.98309178744</v>
-      </c>
-      <c r="L25">
-        <v>11</v>
-      </c>
       <c r="M25">
-        <v>1453082.590909091</v>
-      </c>
-      <c r="N25">
-        <v>6</v>
-      </c>
-      <c r="O25">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
@@ -1714,49 +1512,41 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
           <t>mississippi</t>
         </is>
       </c>
+      <c r="C26">
+        <v>27832636</v>
+      </c>
       <c r="D26">
-        <v>49</v>
+        <v>2781</v>
       </c>
       <c r="E26">
-        <v>27832636</v>
+        <v>10008.13951815894</v>
       </c>
       <c r="F26">
         <v>2986530</v>
       </c>
       <c r="G26">
-        <v>2469</v>
+        <v>9.319389391702076</v>
       </c>
       <c r="H26">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="I26">
-        <v>9.319389391702076</v>
+        <v>29</v>
       </c>
       <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>34</v>
+      </c>
+      <c r="L26">
         <v>17</v>
       </c>
-      <c r="K26">
-        <v>11272.83758606723</v>
-      </c>
-      <c r="L26">
-        <v>32</v>
-      </c>
       <c r="M26">
-        <v>335332.9638554217</v>
-      </c>
-      <c r="N26">
-        <v>34</v>
-      </c>
-      <c r="O26">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
@@ -1767,49 +1557,41 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MO</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
           <t>missouri</t>
         </is>
       </c>
+      <c r="C27">
+        <v>48834120</v>
+      </c>
       <c r="D27">
-        <v>82</v>
+        <v>4469</v>
       </c>
       <c r="E27">
-        <v>49366834</v>
+        <v>10927.3036473484</v>
       </c>
       <c r="F27">
         <v>6126452</v>
       </c>
       <c r="G27">
-        <v>3624</v>
+        <v>7.971027929379027</v>
       </c>
       <c r="H27">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="I27">
-        <v>8.057981030456126</v>
+        <v>26</v>
       </c>
       <c r="J27">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="K27">
-        <v>13622.19481236203</v>
+        <v>18</v>
       </c>
       <c r="L27">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M27">
-        <v>836726</v>
-      </c>
-      <c r="N27">
-        <v>12</v>
-      </c>
-      <c r="O27">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1820,49 +1602,41 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MT</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
           <t>montana</t>
         </is>
       </c>
+      <c r="C28">
+        <v>19337900</v>
+      </c>
       <c r="D28">
-        <v>51</v>
+        <v>387</v>
       </c>
       <c r="E28">
-        <v>19337900</v>
+        <v>49968.7338501292</v>
       </c>
       <c r="F28">
         <v>1062305</v>
       </c>
       <c r="G28">
-        <v>354</v>
+        <v>18.20371738813241</v>
       </c>
       <c r="H28">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I28">
-        <v>18.20371738813241</v>
+        <v>3</v>
       </c>
       <c r="J28">
+        <v>45</v>
+      </c>
+      <c r="K28">
+        <v>43</v>
+      </c>
+      <c r="L28">
         <v>4</v>
       </c>
-      <c r="K28">
-        <v>54626.83615819209</v>
-      </c>
-      <c r="L28">
-        <v>3</v>
-      </c>
       <c r="M28">
-        <v>585996.9696969697</v>
-      </c>
-      <c r="N28">
-        <v>23</v>
-      </c>
-      <c r="O28">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29">
@@ -1873,49 +1647,41 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NE</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
           <t>nebraska</t>
         </is>
       </c>
+      <c r="C29">
+        <v>15660506</v>
+      </c>
       <c r="D29">
-        <v>29</v>
+        <v>814</v>
       </c>
       <c r="E29">
-        <v>15660506</v>
+        <v>19238.95085995086</v>
       </c>
       <c r="F29">
         <v>1929268</v>
       </c>
       <c r="G29">
-        <v>577</v>
+        <v>8.117330510846601</v>
       </c>
       <c r="H29">
+        <v>42</v>
+      </c>
+      <c r="I29">
+        <v>12</v>
+      </c>
+      <c r="J29">
         <v>30</v>
       </c>
-      <c r="I29">
-        <v>8.117330510846601</v>
-      </c>
-      <c r="J29">
+      <c r="K29">
+        <v>37</v>
+      </c>
+      <c r="L29">
         <v>26</v>
       </c>
-      <c r="K29">
-        <v>27141.2582322357</v>
-      </c>
-      <c r="L29">
-        <v>10</v>
-      </c>
       <c r="M29">
-        <v>522016.8666666666</v>
-      </c>
-      <c r="N29">
-        <v>28</v>
-      </c>
-      <c r="O29">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -1926,49 +1692,41 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NV</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
           <t>nevada</t>
         </is>
       </c>
+      <c r="C30">
+        <v>15951518</v>
+      </c>
       <c r="D30">
-        <v>39</v>
+        <v>2836</v>
       </c>
       <c r="E30">
-        <v>15951518</v>
+        <v>5624.653737658674</v>
       </c>
       <c r="F30">
         <v>3034392</v>
       </c>
       <c r="G30">
-        <v>2493</v>
+        <v>5.2569074793237</v>
       </c>
       <c r="H30">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="I30">
-        <v>5.2569074793237</v>
+        <v>40</v>
       </c>
       <c r="J30">
+        <v>14</v>
+      </c>
+      <c r="K30">
+        <v>32</v>
+      </c>
+      <c r="L30">
         <v>50</v>
       </c>
-      <c r="K30">
-        <v>6398.523064580826</v>
-      </c>
-      <c r="L30">
-        <v>42</v>
-      </c>
       <c r="M30">
-        <v>194530.7073170732</v>
-      </c>
-      <c r="N30">
-        <v>43</v>
-      </c>
-      <c r="O30">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
@@ -1979,49 +1737,41 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NH</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
           <t>new hampshire</t>
         </is>
       </c>
+      <c r="C31">
+        <v>13838597</v>
+      </c>
       <c r="D31">
-        <v>26</v>
+        <v>985</v>
       </c>
       <c r="E31">
-        <v>13838597</v>
+        <v>14049.33705583756</v>
       </c>
       <c r="F31">
         <v>1356458</v>
       </c>
       <c r="G31">
-        <v>819</v>
+        <v>10.20200920338116</v>
       </c>
       <c r="H31">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="I31">
-        <v>10.20200920338116</v>
+        <v>19</v>
       </c>
       <c r="J31">
+        <v>22</v>
+      </c>
+      <c r="K31">
+        <v>41</v>
+      </c>
+      <c r="L31">
         <v>14</v>
       </c>
-      <c r="K31">
-        <v>16896.94383394384</v>
-      </c>
-      <c r="L31">
-        <v>19</v>
-      </c>
       <c r="M31">
-        <v>230643.2833333333</v>
-      </c>
-      <c r="N31">
-        <v>40</v>
-      </c>
-      <c r="O31">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
@@ -2032,49 +1782,41 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>NJ</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
           <t>new jersey</t>
         </is>
       </c>
+      <c r="C32">
+        <v>55524423</v>
+      </c>
       <c r="D32">
-        <v>76</v>
+        <v>61850</v>
       </c>
       <c r="E32">
-        <v>55524423</v>
+        <v>897.7271301535974</v>
       </c>
       <c r="F32">
         <v>8908520</v>
       </c>
       <c r="G32">
-        <v>54588</v>
+        <v>6.232732597558292</v>
       </c>
       <c r="H32">
-        <v>613</v>
+        <v>2</v>
       </c>
       <c r="I32">
-        <v>6.232732597558292</v>
+        <v>50</v>
       </c>
       <c r="J32">
+        <v>48</v>
+      </c>
+      <c r="K32">
+        <v>11</v>
+      </c>
+      <c r="L32">
         <v>44</v>
       </c>
-      <c r="K32">
-        <v>1017.154374587822</v>
-      </c>
-      <c r="L32">
-        <v>50</v>
-      </c>
       <c r="M32">
-        <v>90578.17781402936</v>
-      </c>
-      <c r="N32">
-        <v>50</v>
-      </c>
-      <c r="O32">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33">
@@ -2085,49 +1827,41 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>NM</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
           <t>new mexico</t>
         </is>
       </c>
+      <c r="C33">
+        <v>31306643</v>
+      </c>
       <c r="D33">
-        <v>75</v>
+        <v>1245</v>
       </c>
       <c r="E33">
-        <v>31306643</v>
+        <v>25145.89799196787</v>
       </c>
       <c r="F33">
         <v>2095428</v>
       </c>
       <c r="G33">
-        <v>989</v>
+        <v>14.94045273805638</v>
       </c>
       <c r="H33">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I33">
-        <v>14.94045273805638</v>
+        <v>9</v>
       </c>
       <c r="J33">
+        <v>31</v>
+      </c>
+      <c r="K33">
+        <v>36</v>
+      </c>
+      <c r="L33">
         <v>8</v>
       </c>
-      <c r="K33">
-        <v>31654.84630940344</v>
-      </c>
-      <c r="L33">
-        <v>9</v>
-      </c>
       <c r="M33">
-        <v>666098.7872340425</v>
-      </c>
-      <c r="N33">
-        <v>19</v>
-      </c>
-      <c r="O33">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34">
@@ -2138,49 +1872,41 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NY</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
           <t>new york</t>
         </is>
       </c>
+      <c r="C34">
+        <v>152607845</v>
+      </c>
       <c r="D34">
-        <v>199</v>
+        <v>190288</v>
       </c>
       <c r="E34">
-        <v>153913967</v>
+        <v>801.9835459934416</v>
       </c>
       <c r="F34">
         <v>19542209</v>
       </c>
       <c r="G34">
-        <v>161807</v>
+        <v>7.809139949327121</v>
       </c>
       <c r="H34">
-        <v>828</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>7.875975894025082</v>
+        <v>51</v>
       </c>
       <c r="J34">
+        <v>50</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="L34">
         <v>30</v>
       </c>
-      <c r="K34">
-        <v>951.2194589850872</v>
-      </c>
-      <c r="L34">
-        <v>51</v>
-      </c>
       <c r="M34">
-        <v>185886.4335748792</v>
-      </c>
-      <c r="N34">
-        <v>44</v>
-      </c>
-      <c r="O34">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35">
@@ -2191,49 +1917,41 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>NC</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
           <t>north carolina</t>
         </is>
       </c>
+      <c r="C35">
+        <v>60229488</v>
+      </c>
       <c r="D35">
-        <v>136</v>
+        <v>4602</v>
       </c>
       <c r="E35">
-        <v>60229488</v>
+        <v>13087.67666232073</v>
       </c>
       <c r="F35">
         <v>10383620</v>
       </c>
       <c r="G35">
-        <v>3962</v>
+        <v>5.800432604428899</v>
       </c>
       <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <v>23</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>9</v>
+      </c>
+      <c r="L35">
+        <v>47</v>
+      </c>
+      <c r="M35">
         <v>38</v>
-      </c>
-      <c r="I35">
-        <v>5.800432604428899</v>
-      </c>
-      <c r="J35">
-        <v>47</v>
-      </c>
-      <c r="K35">
-        <v>15201.78899545684</v>
-      </c>
-      <c r="L35">
-        <v>23</v>
-      </c>
-      <c r="M35">
-        <v>1584986.526315789</v>
-      </c>
-      <c r="N35">
-        <v>4</v>
-      </c>
-      <c r="O35">
-        <v>41</v>
       </c>
     </row>
     <row r="36">
@@ -2244,49 +1962,41 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
           <t>north dakota</t>
         </is>
       </c>
+      <c r="C36">
+        <v>9641944</v>
+      </c>
       <c r="D36">
-        <v>19</v>
+        <v>308</v>
       </c>
       <c r="E36">
-        <v>9641944</v>
+        <v>31305.01298701299</v>
       </c>
       <c r="F36">
         <v>760077</v>
       </c>
       <c r="G36">
-        <v>269</v>
+        <v>12.68548318130926</v>
       </c>
       <c r="H36">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I36">
-        <v>12.68548318130926</v>
+        <v>7</v>
       </c>
       <c r="J36">
+        <v>42</v>
+      </c>
+      <c r="K36">
+        <v>47</v>
+      </c>
+      <c r="L36">
         <v>11</v>
       </c>
-      <c r="K36">
-        <v>35843.65799256506</v>
-      </c>
-      <c r="L36">
-        <v>7</v>
-      </c>
       <c r="M36">
-        <v>275484.1142857143</v>
-      </c>
-      <c r="N36">
-        <v>37</v>
-      </c>
-      <c r="O36">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37">
@@ -2297,49 +2007,41 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>OH</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
           <t>ohio</t>
         </is>
       </c>
+      <c r="C37">
+        <v>76966291</v>
+      </c>
       <c r="D37">
-        <v>130</v>
+        <v>6604</v>
       </c>
       <c r="E37">
-        <v>76966291</v>
+        <v>11654.49591156875</v>
       </c>
       <c r="F37">
         <v>11689442</v>
       </c>
       <c r="G37">
-        <v>5512</v>
+        <v>6.584257058634621</v>
       </c>
       <c r="H37">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I37">
-        <v>6.584257058634621</v>
+        <v>25</v>
       </c>
       <c r="J37">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="K37">
-        <v>13963.40547895501</v>
+        <v>7</v>
       </c>
       <c r="L37">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="M37">
-        <v>1637580.659574468</v>
-      </c>
-      <c r="N37">
-        <v>3</v>
-      </c>
-      <c r="O37">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
@@ -2350,49 +2052,41 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
           <t>oklahoma</t>
         </is>
       </c>
+      <c r="C38">
+        <v>35271126</v>
+      </c>
       <c r="D38">
-        <v>89</v>
+        <v>1970</v>
       </c>
       <c r="E38">
-        <v>35271126</v>
+        <v>17904.12487309645</v>
       </c>
       <c r="F38">
         <v>3943079</v>
       </c>
       <c r="G38">
-        <v>1686</v>
+        <v>8.945072112427877</v>
       </c>
       <c r="H38">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="I38">
-        <v>8.945072112427877</v>
+        <v>14</v>
       </c>
       <c r="J38">
+        <v>17</v>
+      </c>
+      <c r="K38">
+        <v>28</v>
+      </c>
+      <c r="L38">
         <v>20</v>
       </c>
-      <c r="K38">
-        <v>20920.00355871886</v>
-      </c>
-      <c r="L38">
-        <v>16</v>
-      </c>
       <c r="M38">
-        <v>820258.7441860465</v>
-      </c>
-      <c r="N38">
-        <v>14</v>
-      </c>
-      <c r="O38">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
@@ -2403,49 +2097,41 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
           <t>oregon</t>
         </is>
       </c>
+      <c r="C39">
+        <v>42445964</v>
+      </c>
       <c r="D39">
-        <v>116</v>
+        <v>1527</v>
       </c>
       <c r="E39">
-        <v>42445964</v>
+        <v>27796.96398166339</v>
       </c>
       <c r="F39">
         <v>4190713</v>
       </c>
       <c r="G39">
-        <v>1322</v>
+        <v>10.12857812023873</v>
       </c>
       <c r="H39">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I39">
-        <v>10.12857812023873</v>
+        <v>8</v>
       </c>
       <c r="J39">
+        <v>28</v>
+      </c>
+      <c r="K39">
+        <v>27</v>
+      </c>
+      <c r="L39">
         <v>15</v>
       </c>
-      <c r="K39">
-        <v>32107.38577912254</v>
-      </c>
-      <c r="L39">
-        <v>8</v>
-      </c>
       <c r="M39">
-        <v>1326436.375</v>
-      </c>
-      <c r="N39">
-        <v>7</v>
-      </c>
-      <c r="O39">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40">
@@ -2456,49 +2142,41 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PA</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
           <t>pennsylvania</t>
         </is>
       </c>
+      <c r="C40">
+        <v>82353417</v>
+      </c>
       <c r="D40">
-        <v>117</v>
+        <v>23036</v>
       </c>
       <c r="E40">
-        <v>82353417</v>
+        <v>3574.987714881056</v>
       </c>
       <c r="F40">
         <v>12807060</v>
       </c>
       <c r="G40">
-        <v>18633</v>
+        <v>6.430313983068714</v>
       </c>
       <c r="H40">
-        <v>145</v>
+        <v>6</v>
       </c>
       <c r="I40">
-        <v>6.430313983068714</v>
+        <v>45</v>
       </c>
       <c r="J40">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K40">
-        <v>4419.76155208501</v>
+        <v>5</v>
       </c>
       <c r="L40">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M40">
-        <v>567954.6</v>
-      </c>
-      <c r="N40">
-        <v>25</v>
-      </c>
-      <c r="O40">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41">
@@ -2509,49 +2187,41 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>RI</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
           <t>rhode island</t>
         </is>
       </c>
+      <c r="C41">
+        <v>15395742</v>
+      </c>
       <c r="D41">
-        <v>26</v>
+        <v>2665</v>
       </c>
       <c r="E41">
-        <v>15395742</v>
+        <v>5777.013883677299</v>
       </c>
       <c r="F41">
         <v>1057315</v>
       </c>
       <c r="G41">
-        <v>1727</v>
+        <v>14.56116862051517</v>
       </c>
       <c r="H41">
-        <v>163</v>
+        <v>28</v>
       </c>
       <c r="I41">
-        <v>14.56116862051517</v>
+        <v>38</v>
       </c>
       <c r="J41">
+        <v>10</v>
+      </c>
+      <c r="K41">
+        <v>44</v>
+      </c>
+      <c r="L41">
         <v>9</v>
       </c>
-      <c r="K41">
-        <v>8914.731905037637</v>
-      </c>
-      <c r="L41">
+      <c r="M41">
         <v>35</v>
-      </c>
-      <c r="M41">
-        <v>94452.40490797546</v>
-      </c>
-      <c r="N41">
-        <v>49</v>
-      </c>
-      <c r="O41">
-        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -2562,49 +2232,41 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
           <t>south carolina</t>
         </is>
       </c>
+      <c r="C42">
+        <v>36151921</v>
+      </c>
       <c r="D42">
-        <v>71</v>
+        <v>3320</v>
       </c>
       <c r="E42">
-        <v>36151921</v>
+        <v>10889.1328313253</v>
       </c>
       <c r="F42">
         <v>5084127</v>
       </c>
       <c r="G42">
-        <v>2793</v>
+        <v>7.11074310299487</v>
       </c>
       <c r="H42">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="I42">
-        <v>7.11074310299487</v>
+        <v>27</v>
       </c>
       <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>23</v>
+      </c>
+      <c r="L42">
         <v>32</v>
       </c>
-      <c r="K42">
-        <v>12943.75975653419</v>
-      </c>
-      <c r="L42">
-        <v>28</v>
-      </c>
       <c r="M42">
-        <v>657307.6545454545</v>
-      </c>
-      <c r="N42">
-        <v>21</v>
-      </c>
-      <c r="O42">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
@@ -2615,49 +2277,41 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
           <t>south dakota</t>
         </is>
       </c>
+      <c r="C43">
+        <v>10231886</v>
+      </c>
       <c r="D43">
-        <v>23</v>
+        <v>730</v>
       </c>
       <c r="E43">
-        <v>10231886</v>
+        <v>14016.28219178082</v>
       </c>
       <c r="F43">
         <v>882235</v>
       </c>
       <c r="G43">
-        <v>447</v>
+        <v>11.59768769092135</v>
       </c>
       <c r="H43">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I43">
-        <v>11.59768769092135</v>
+        <v>20</v>
       </c>
       <c r="J43">
+        <v>24</v>
+      </c>
+      <c r="K43">
+        <v>46</v>
+      </c>
+      <c r="L43">
         <v>12</v>
       </c>
-      <c r="K43">
-        <v>22890.12527964206</v>
-      </c>
-      <c r="L43">
-        <v>14</v>
-      </c>
       <c r="M43">
-        <v>200625.2156862745</v>
-      </c>
-      <c r="N43">
-        <v>42</v>
-      </c>
-      <c r="O43">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44">
@@ -2668,49 +2322,41 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TN</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
           <t>tennessee</t>
         </is>
       </c>
+      <c r="C44">
+        <v>53160247</v>
+      </c>
       <c r="D44">
-        <v>92</v>
+        <v>5508</v>
       </c>
       <c r="E44">
-        <v>53352585</v>
+        <v>9651.460965867829</v>
       </c>
       <c r="F44">
         <v>6770010</v>
       </c>
       <c r="G44">
-        <v>4634</v>
+        <v>7.852314398353917</v>
       </c>
       <c r="H44">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="I44">
-        <v>7.880724696123049</v>
+        <v>30</v>
       </c>
       <c r="J44">
+        <v>11</v>
+      </c>
+      <c r="K44">
+        <v>16</v>
+      </c>
+      <c r="L44">
         <v>29</v>
       </c>
-      <c r="K44">
-        <v>11513.28981441519</v>
-      </c>
-      <c r="L44">
-        <v>31</v>
-      </c>
       <c r="M44">
-        <v>784596.8382352941</v>
-      </c>
-      <c r="N44">
-        <v>16</v>
-      </c>
-      <c r="O44">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
@@ -2721,49 +2367,41 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
           <t>texas</t>
         </is>
       </c>
+      <c r="C45">
+        <v>162768263</v>
+      </c>
       <c r="D45">
-        <v>216</v>
+        <v>13886</v>
       </c>
       <c r="E45">
-        <v>163123763</v>
+        <v>11721.75306063661</v>
       </c>
       <c r="F45">
         <v>28701845</v>
       </c>
       <c r="G45">
-        <v>11483</v>
+        <v>5.671003484270785</v>
       </c>
       <c r="H45">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="I45">
-        <v>5.683389447612166</v>
+        <v>24</v>
       </c>
       <c r="J45">
+        <v>14</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
         <v>49</v>
       </c>
-      <c r="K45">
-        <v>14205.6747365671</v>
-      </c>
-      <c r="L45">
-        <v>24</v>
-      </c>
       <c r="M45">
-        <v>4078094.075</v>
-      </c>
-      <c r="N45">
-        <v>2</v>
-      </c>
-      <c r="O45">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46">
@@ -2774,49 +2412,41 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>UT</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
           <t>utah</t>
         </is>
       </c>
+      <c r="C46">
+        <v>20897088</v>
+      </c>
       <c r="D46">
-        <v>37</v>
+        <v>2303</v>
       </c>
       <c r="E46">
-        <v>20897088</v>
+        <v>9073.854971775945</v>
       </c>
       <c r="F46">
         <v>3161105</v>
       </c>
       <c r="G46">
-        <v>1977</v>
+        <v>6.610690881827716</v>
       </c>
       <c r="H46">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="I46">
-        <v>6.610690881827716</v>
+        <v>32</v>
       </c>
       <c r="J46">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="K46">
-        <v>10570.10015174507</v>
+        <v>30</v>
       </c>
       <c r="L46">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="M46">
-        <v>331699.8095238095</v>
-      </c>
-      <c r="N46">
-        <v>35</v>
-      </c>
-      <c r="O46">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
@@ -2827,49 +2457,41 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>VT</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
           <t>vermont</t>
         </is>
       </c>
+      <c r="C47">
+        <v>15697419</v>
+      </c>
       <c r="D47">
-        <v>31</v>
+        <v>748</v>
       </c>
       <c r="E47">
-        <v>15697419</v>
+        <v>20985.85427807487</v>
       </c>
       <c r="F47">
         <v>626299</v>
       </c>
       <c r="G47">
-        <v>679</v>
+        <v>25.06377784412876</v>
       </c>
       <c r="H47">
-        <v>108</v>
+        <v>43</v>
       </c>
       <c r="I47">
-        <v>25.06377784412876</v>
+        <v>10</v>
       </c>
       <c r="J47">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="K47">
-        <v>23118.43740795287</v>
+        <v>50</v>
       </c>
       <c r="L47">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M47">
-        <v>145346.4722222222</v>
-      </c>
-      <c r="N47">
-        <v>45</v>
-      </c>
-      <c r="O47">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48">
@@ -2880,49 +2502,41 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>VA</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
           <t>virginia</t>
         </is>
       </c>
+      <c r="C48">
+        <v>43497577</v>
+      </c>
       <c r="D48">
-        <v>71</v>
+        <v>5747</v>
       </c>
       <c r="E48">
-        <v>43497577</v>
+        <v>7568.744910388029</v>
       </c>
       <c r="F48">
         <v>8517685</v>
       </c>
       <c r="G48">
-        <v>4509</v>
+        <v>5.106736983112196</v>
       </c>
       <c r="H48">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="I48">
-        <v>5.106736983112196</v>
+        <v>34</v>
       </c>
       <c r="J48">
+        <v>16</v>
+      </c>
+      <c r="K48">
+        <v>12</v>
+      </c>
+      <c r="L48">
         <v>51</v>
       </c>
-      <c r="K48">
-        <v>9646.83455311599</v>
-      </c>
-      <c r="L48">
-        <v>34</v>
-      </c>
       <c r="M48">
-        <v>820709</v>
-      </c>
-      <c r="N48">
-        <v>13</v>
-      </c>
-      <c r="O48">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49">
@@ -2933,49 +2547,41 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>WA</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
           <t>washington</t>
         </is>
       </c>
+      <c r="C49">
+        <v>65424260</v>
+      </c>
       <c r="D49">
-        <v>122</v>
+        <v>10609</v>
       </c>
       <c r="E49">
-        <v>65424260</v>
+        <v>6166.863983410312</v>
       </c>
       <c r="F49">
         <v>7535591</v>
       </c>
       <c r="G49">
-        <v>9753</v>
+        <v>8.682034362002927</v>
       </c>
       <c r="H49">
-        <v>129</v>
+        <v>13</v>
       </c>
       <c r="I49">
-        <v>8.682034362002927</v>
+        <v>37</v>
       </c>
       <c r="J49">
+        <v>24</v>
+      </c>
+      <c r="K49">
+        <v>13</v>
+      </c>
+      <c r="L49">
         <v>21</v>
       </c>
-      <c r="K49">
-        <v>6708.116476981441</v>
-      </c>
-      <c r="L49">
-        <v>39</v>
-      </c>
       <c r="M49">
-        <v>507164.8062015504</v>
-      </c>
-      <c r="N49">
-        <v>29</v>
-      </c>
-      <c r="O49">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -2986,49 +2592,41 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>WV</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
           <t>west virginia</t>
         </is>
       </c>
+      <c r="C50">
+        <v>30983620</v>
+      </c>
       <c r="D50">
-        <v>67</v>
+        <v>611</v>
       </c>
       <c r="E50">
-        <v>30983620</v>
+        <v>50709.68903436988</v>
       </c>
       <c r="F50">
         <v>1805832</v>
       </c>
       <c r="G50">
-        <v>536</v>
+        <v>17.15753181912825</v>
       </c>
       <c r="H50">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="I50">
-        <v>17.15753181912825</v>
+        <v>2</v>
       </c>
       <c r="J50">
+        <v>44</v>
+      </c>
+      <c r="K50">
+        <v>38</v>
+      </c>
+      <c r="L50">
         <v>6</v>
       </c>
-      <c r="K50">
-        <v>57805.26119402985</v>
-      </c>
-      <c r="L50">
-        <v>2</v>
-      </c>
       <c r="M50">
-        <v>1032787.333333333</v>
-      </c>
-      <c r="N50">
-        <v>10</v>
-      </c>
-      <c r="O50">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51">
@@ -3039,49 +2637,41 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>WI</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
           <t>wisconsin</t>
         </is>
       </c>
+      <c r="C51">
+        <v>35249718</v>
+      </c>
       <c r="D51">
-        <v>57</v>
+        <v>3341</v>
       </c>
       <c r="E51">
-        <v>35249718</v>
+        <v>10550.64890751272</v>
       </c>
       <c r="F51">
         <v>5813568</v>
       </c>
       <c r="G51">
-        <v>2890</v>
+        <v>6.063353520591829</v>
       </c>
       <c r="H51">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="I51">
-        <v>6.063353520591829</v>
+        <v>28</v>
       </c>
       <c r="J51">
+        <v>4</v>
+      </c>
+      <c r="K51">
+        <v>20</v>
+      </c>
+      <c r="L51">
         <v>45</v>
       </c>
-      <c r="K51">
-        <v>12197.13425605536</v>
-      </c>
-      <c r="L51">
-        <v>29</v>
-      </c>
       <c r="M51">
-        <v>704994.36</v>
-      </c>
-      <c r="N51">
-        <v>17</v>
-      </c>
-      <c r="O51">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52">
@@ -3092,49 +2682,41 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>WY</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
           <t>wyoming</t>
         </is>
       </c>
+      <c r="C52">
+        <v>10194407</v>
+      </c>
       <c r="D52">
-        <v>19</v>
+        <v>270</v>
       </c>
       <c r="E52">
-        <v>10194407</v>
+        <v>37757.06296296296</v>
       </c>
       <c r="F52">
         <v>577737</v>
       </c>
       <c r="G52">
-        <v>239</v>
+        <v>17.64541132037588</v>
       </c>
       <c r="H52">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I52">
-        <v>17.64541132037588</v>
+        <v>5</v>
       </c>
       <c r="J52">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="K52">
-        <v>42654.42259414226</v>
+        <v>51</v>
       </c>
       <c r="L52">
         <v>5</v>
       </c>
       <c r="M52">
-        <v>248644.0731707317</v>
-      </c>
-      <c r="N52">
-        <v>38</v>
-      </c>
-      <c r="O52">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with new data files
</commit_message>
<xml_diff>
--- a/output/joined_taggs_bystate.xlsx
+++ b/output/joined_taggs_bystate.xlsx
@@ -436,37 +436,37 @@
         </is>
       </c>
       <c r="C2">
-        <v>34117522</v>
+        <v>99441675</v>
       </c>
       <c r="D2">
-        <v>3611</v>
+        <v>4946</v>
       </c>
       <c r="E2">
-        <v>9448.219883688729</v>
+        <v>20105.47412050141</v>
       </c>
       <c r="F2">
-        <v>4874747</v>
+        <v>4887871</v>
       </c>
       <c r="G2">
-        <v>6.998829272575582</v>
+        <v>20.34457844734446</v>
       </c>
       <c r="H2">
         <v>22</v>
       </c>
       <c r="I2">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K2">
         <v>24</v>
       </c>
       <c r="L2">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="M2">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -481,19 +481,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>30295475</v>
+        <v>42943025</v>
       </c>
       <c r="D3">
-        <v>272</v>
+        <v>319</v>
       </c>
       <c r="E3">
-        <v>111380.4227941177</v>
+        <v>134617.6332288401</v>
       </c>
       <c r="F3">
-        <v>739795</v>
+        <v>737438</v>
       </c>
       <c r="G3">
-        <v>40.95117566352841</v>
+        <v>58.23272600544046</v>
       </c>
       <c r="H3">
         <v>50</v>
@@ -526,37 +526,37 @@
         </is>
       </c>
       <c r="C4">
-        <v>49778142</v>
+        <v>156118344</v>
       </c>
       <c r="D4">
-        <v>3542</v>
+        <v>4933</v>
       </c>
       <c r="E4">
-        <v>14053.68210050819</v>
+        <v>31647.7486316643</v>
       </c>
       <c r="F4">
-        <v>7016270</v>
+        <v>7171646</v>
       </c>
       <c r="G4">
-        <v>7.094673095533667</v>
+        <v>21.76883019602473</v>
       </c>
       <c r="H4">
         <v>23</v>
       </c>
       <c r="I4">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K4">
         <v>14</v>
       </c>
       <c r="L4">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="M4">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -571,37 +571,37 @@
         </is>
       </c>
       <c r="C5">
-        <v>20471146</v>
+        <v>63313280</v>
       </c>
       <c r="D5">
-        <v>1398</v>
+        <v>1853</v>
       </c>
       <c r="E5">
-        <v>14643.16595135908</v>
+        <v>34167.98704803022</v>
       </c>
       <c r="F5">
-        <v>3004279</v>
+        <v>3013825</v>
       </c>
       <c r="G5">
-        <v>6.813996303272766</v>
+        <v>21.00761656698714</v>
       </c>
       <c r="H5">
         <v>38</v>
       </c>
       <c r="I5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J5">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L5">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -616,37 +616,37 @@
         </is>
       </c>
       <c r="C6">
-        <v>329575212</v>
+        <v>695469251</v>
       </c>
       <c r="D6">
-        <v>23324</v>
+        <v>31531</v>
       </c>
       <c r="E6">
-        <v>14130.30406448294</v>
+        <v>22056.68234435952</v>
       </c>
       <c r="F6">
-        <v>39536653</v>
+        <v>39557045</v>
       </c>
       <c r="G6">
-        <v>8.335941132902676</v>
+        <v>17.58142578648127</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
       <c r="I6">
+        <v>22</v>
+      </c>
+      <c r="J6">
         <v>17</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M6">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -661,37 +661,37 @@
         </is>
       </c>
       <c r="C7">
-        <v>46734343</v>
+        <v>91392178</v>
       </c>
       <c r="D7">
-        <v>7307</v>
+        <v>9730</v>
       </c>
       <c r="E7">
-        <v>6395.83180511838</v>
+        <v>9392.824049331963</v>
       </c>
       <c r="F7">
-        <v>5607154</v>
+        <v>5695564</v>
       </c>
       <c r="G7">
-        <v>8.334770723258181</v>
+        <v>16.04620332595683</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K7">
         <v>21</v>
       </c>
       <c r="L7">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="M7">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -706,37 +706,37 @@
         </is>
       </c>
       <c r="C8">
-        <v>33012783</v>
+        <v>57701322</v>
       </c>
       <c r="D8">
-        <v>12035</v>
+        <v>17962</v>
       </c>
       <c r="E8">
-        <v>2743.064644786041</v>
+        <v>3212.41075604053</v>
       </c>
       <c r="F8">
-        <v>3588184</v>
+        <v>3572665</v>
       </c>
       <c r="G8">
-        <v>9.200415307576201</v>
+        <v>16.15077876039315</v>
       </c>
       <c r="H8">
         <v>12</v>
       </c>
       <c r="I8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K8">
         <v>29</v>
       </c>
       <c r="L8">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="M8">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -751,37 +751,37 @@
         </is>
       </c>
       <c r="C9">
-        <v>8882569</v>
+        <v>19276224</v>
       </c>
       <c r="D9">
-        <v>1625</v>
+        <v>2538</v>
       </c>
       <c r="E9">
-        <v>5466.196307692308</v>
+        <v>7595.044917257684</v>
       </c>
       <c r="F9">
-        <v>961939</v>
+        <v>967171</v>
       </c>
       <c r="G9">
-        <v>9.234025234448339</v>
+        <v>19.93052314430437</v>
       </c>
       <c r="H9">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I9">
         <v>41</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9">
         <v>45</v>
       </c>
       <c r="L9">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M9">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -796,37 +796,37 @@
         </is>
       </c>
       <c r="C10">
-        <v>15905496</v>
+        <v>24261074</v>
       </c>
       <c r="D10">
-        <v>1875</v>
+        <v>2927</v>
       </c>
       <c r="E10">
-        <v>8482.931200000001</v>
+        <v>8288.7167748548</v>
       </c>
       <c r="F10">
-        <v>693972</v>
+        <v>702455</v>
       </c>
       <c r="G10">
-        <v>22.91950683889263</v>
+        <v>34.53754902449267</v>
       </c>
       <c r="H10">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K10">
         <v>49</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -841,37 +841,37 @@
         </is>
       </c>
       <c r="C11">
-        <v>128572709</v>
+        <v>362359635</v>
       </c>
       <c r="D11">
-        <v>19895</v>
+        <v>26660</v>
       </c>
       <c r="E11">
-        <v>6462.563910530284</v>
+        <v>13591.88428357089</v>
       </c>
       <c r="F11">
-        <v>20984400</v>
+        <v>21299325</v>
       </c>
       <c r="G11">
-        <v>6.127061483768895</v>
+        <v>17.01272857238434</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I11">
         <v>35</v>
       </c>
       <c r="J11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
       <c r="L11">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M11">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -886,37 +886,37 @@
         </is>
       </c>
       <c r="C12">
-        <v>66962578</v>
+        <v>262844797</v>
       </c>
       <c r="D12">
-        <v>12550</v>
+        <v>18499</v>
       </c>
       <c r="E12">
-        <v>5335.66358565737</v>
+        <v>14208.59489702146</v>
       </c>
       <c r="F12">
-        <v>10429379</v>
+        <v>10519475</v>
       </c>
       <c r="G12">
-        <v>6.420571924752183</v>
+        <v>24.98649381266651</v>
       </c>
       <c r="H12">
         <v>11</v>
       </c>
       <c r="I12">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="J12">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="K12">
         <v>8</v>
       </c>
       <c r="L12">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="M12">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -931,37 +931,37 @@
         </is>
       </c>
       <c r="C13">
-        <v>19630770</v>
+        <v>32028211</v>
       </c>
       <c r="D13">
-        <v>499</v>
+        <v>580</v>
       </c>
       <c r="E13">
-        <v>39340.22044088176</v>
+        <v>55221.05344827586</v>
       </c>
       <c r="F13">
-        <v>1427538</v>
+        <v>1420491</v>
       </c>
       <c r="G13">
-        <v>13.75148682556962</v>
+        <v>22.54728189055756</v>
       </c>
       <c r="H13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I13">
         <v>4</v>
       </c>
       <c r="J13">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13">
         <v>40</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="M13">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
@@ -976,37 +976,37 @@
         </is>
       </c>
       <c r="C14">
-        <v>19050242</v>
+        <v>40943191</v>
       </c>
       <c r="D14">
-        <v>1426</v>
+        <v>1672</v>
       </c>
       <c r="E14">
-        <v>13359.2159887798</v>
+        <v>24487.55442583732</v>
       </c>
       <c r="F14">
-        <v>1716943</v>
+        <v>1754208</v>
       </c>
       <c r="G14">
-        <v>11.09544230647144</v>
+        <v>23.33998647822835</v>
       </c>
       <c r="H14">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I14">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K14">
         <v>39</v>
       </c>
       <c r="L14">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M14">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
@@ -1021,37 +1021,37 @@
         </is>
       </c>
       <c r="C15">
-        <v>102146038</v>
+        <v>226300406</v>
       </c>
       <c r="D15">
-        <v>20852</v>
+        <v>30357</v>
       </c>
       <c r="E15">
-        <v>4898.620659888739</v>
+        <v>7454.636690055012</v>
       </c>
       <c r="F15">
-        <v>12802023</v>
+        <v>12741080</v>
       </c>
       <c r="G15">
-        <v>7.978898178826893</v>
+        <v>17.76147751995906</v>
       </c>
       <c r="H15">
         <v>7</v>
       </c>
       <c r="I15">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15">
         <v>6</v>
       </c>
       <c r="L15">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="M15">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -1066,37 +1066,37 @@
         </is>
       </c>
       <c r="C16">
-        <v>45762425</v>
+        <v>126439063</v>
       </c>
       <c r="D16">
-        <v>7928</v>
+        <v>11211</v>
       </c>
       <c r="E16">
-        <v>5772.253405650858</v>
+        <v>11278.12532334315</v>
       </c>
       <c r="F16">
-        <v>6666818</v>
+        <v>6691878</v>
       </c>
       <c r="G16">
-        <v>6.864207932479933</v>
+        <v>18.8944064730409</v>
       </c>
       <c r="H16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I16">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J16">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K16">
         <v>17</v>
       </c>
       <c r="L16">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M16">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -1111,37 +1111,37 @@
         </is>
       </c>
       <c r="C17">
-        <v>22061848</v>
+        <v>55287159</v>
       </c>
       <c r="D17">
-        <v>1587</v>
+        <v>2902</v>
       </c>
       <c r="E17">
-        <v>13901.60554505356</v>
+        <v>19051.39869055824</v>
       </c>
       <c r="F17">
-        <v>3145711</v>
+        <v>3156145</v>
       </c>
       <c r="G17">
-        <v>7.013310504366103</v>
+        <v>17.51730639751976</v>
       </c>
       <c r="H17">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I17">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J17">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="K17">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L17">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1156,37 +1156,37 @@
         </is>
       </c>
       <c r="C18">
-        <v>25194340</v>
+        <v>57159679</v>
       </c>
       <c r="D18">
-        <v>1344</v>
+        <v>1949</v>
       </c>
       <c r="E18">
-        <v>18745.78869047619</v>
+        <v>29327.69574140585</v>
       </c>
       <c r="F18">
-        <v>2913123</v>
+        <v>2911510</v>
       </c>
       <c r="G18">
-        <v>8.648567190606096</v>
+        <v>19.63231416000632</v>
       </c>
       <c r="H18">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I18">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J18">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K18">
         <v>35</v>
       </c>
       <c r="L18">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M18">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -1201,37 +1201,37 @@
         </is>
       </c>
       <c r="C19">
-        <v>34508140</v>
+        <v>103947049</v>
       </c>
       <c r="D19">
-        <v>2018</v>
+        <v>2960</v>
       </c>
       <c r="E19">
-        <v>17100.16848364718</v>
+        <v>35117.24628378378</v>
       </c>
       <c r="F19">
-        <v>4454189</v>
+        <v>4468402</v>
       </c>
       <c r="G19">
-        <v>7.747345251851684</v>
+        <v>23.26268965952481</v>
       </c>
       <c r="H19">
         <v>30</v>
       </c>
       <c r="I19">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J19">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K19">
         <v>26</v>
       </c>
       <c r="L19">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="M19">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -1246,37 +1246,37 @@
         </is>
       </c>
       <c r="C20">
-        <v>43767117</v>
+        <v>114820913</v>
       </c>
       <c r="D20">
-        <v>20595</v>
+        <v>23928</v>
       </c>
       <c r="E20">
-        <v>2125.133139111435</v>
+        <v>4798.600509862922</v>
       </c>
       <c r="F20">
-        <v>4684333</v>
+        <v>4659978</v>
       </c>
       <c r="G20">
-        <v>9.343297540973282</v>
+        <v>24.63979722651051</v>
       </c>
       <c r="H20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I20">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J20">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K20">
         <v>25</v>
       </c>
       <c r="L20">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="M20">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -1291,37 +1291,37 @@
         </is>
       </c>
       <c r="C21">
-        <v>20145464</v>
+        <v>31957402</v>
       </c>
       <c r="D21">
-        <v>633</v>
+        <v>867</v>
       </c>
       <c r="E21">
-        <v>31825.3775671406</v>
+        <v>36859.74855824683</v>
       </c>
       <c r="F21">
-        <v>1335907</v>
+        <v>1338404</v>
       </c>
       <c r="G21">
-        <v>15.07998984959282</v>
+        <v>23.87724633219865</v>
       </c>
       <c r="H21">
         <v>45</v>
       </c>
       <c r="I21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J21">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K21">
         <v>42</v>
       </c>
       <c r="L21">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M21">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22">
@@ -1336,25 +1336,25 @@
         </is>
       </c>
       <c r="C22">
-        <v>39760392</v>
+        <v>88579941</v>
       </c>
       <c r="D22">
-        <v>8936</v>
+        <v>13700</v>
       </c>
       <c r="E22">
-        <v>4449.461951656222</v>
+        <v>6465.689124087591</v>
       </c>
       <c r="F22">
-        <v>6052177</v>
+        <v>6042718</v>
       </c>
       <c r="G22">
-        <v>6.569601649125596</v>
+        <v>14.65895661521852</v>
       </c>
       <c r="H22">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I22">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J22">
         <v>30</v>
@@ -1363,10 +1363,10 @@
         <v>19</v>
       </c>
       <c r="L22">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="M22">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
@@ -1381,37 +1381,37 @@
         </is>
       </c>
       <c r="C23">
-        <v>59655700</v>
+        <v>109899595</v>
       </c>
       <c r="D23">
-        <v>25475</v>
+        <v>38077</v>
       </c>
       <c r="E23">
-        <v>2341.7350343474</v>
+        <v>2886.246159098669</v>
       </c>
       <c r="F23">
-        <v>6859819</v>
+        <v>6902149</v>
       </c>
       <c r="G23">
-        <v>8.696395633762348</v>
+        <v>15.92251847938953</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
       <c r="I23">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J23">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K23">
         <v>15</v>
       </c>
       <c r="L23">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="M23">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
@@ -1426,37 +1426,37 @@
         </is>
       </c>
       <c r="C24">
-        <v>66563270</v>
+        <v>171051203</v>
       </c>
       <c r="D24">
-        <v>24244</v>
+        <v>31424</v>
       </c>
       <c r="E24">
-        <v>2745.556426332289</v>
+        <v>5443.330034368635</v>
       </c>
       <c r="F24">
-        <v>9962311</v>
+        <v>9995915</v>
       </c>
       <c r="G24">
-        <v>6.68150893904035</v>
+        <v>17.11211059717895</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I24">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K24">
         <v>10</v>
       </c>
       <c r="L24">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M24">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25">
@@ -1471,37 +1471,37 @@
         </is>
       </c>
       <c r="C25">
-        <v>31967817</v>
+        <v>83932128</v>
       </c>
       <c r="D25">
-        <v>1621</v>
+        <v>2356</v>
       </c>
       <c r="E25">
-        <v>19721.04688463911</v>
+        <v>35624.84210526316</v>
       </c>
       <c r="F25">
-        <v>5576606</v>
+        <v>5611179</v>
       </c>
       <c r="G25">
-        <v>5.732486211147067</v>
+        <v>14.95802005247026</v>
       </c>
       <c r="H25">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I25">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J25">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K25">
         <v>22</v>
       </c>
       <c r="L25">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M25">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
@@ -1516,19 +1516,19 @@
         </is>
       </c>
       <c r="C26">
-        <v>27832636</v>
+        <v>76895835</v>
       </c>
       <c r="D26">
-        <v>2781</v>
+        <v>4274</v>
       </c>
       <c r="E26">
-        <v>10008.13951815894</v>
+        <v>17991.5383715489</v>
       </c>
       <c r="F26">
-        <v>2984100</v>
+        <v>2986530</v>
       </c>
       <c r="G26">
-        <v>9.326978318420965</v>
+        <v>25.74755150626312</v>
       </c>
       <c r="H26">
         <v>27</v>
@@ -1543,10 +1543,10 @@
         <v>34</v>
       </c>
       <c r="L26">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M26">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
@@ -1561,37 +1561,37 @@
         </is>
       </c>
       <c r="C27">
-        <v>48834120</v>
+        <v>118943084</v>
       </c>
       <c r="D27">
-        <v>4469</v>
+        <v>5807</v>
       </c>
       <c r="E27">
-        <v>10927.3036473484</v>
+        <v>20482.70776648872</v>
       </c>
       <c r="F27">
-        <v>6113532</v>
+        <v>6126452</v>
       </c>
       <c r="G27">
-        <v>7.987873458419781</v>
+        <v>19.41467655341134</v>
       </c>
       <c r="H27">
         <v>21</v>
       </c>
       <c r="I27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K27">
         <v>18</v>
       </c>
       <c r="L27">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M27">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
@@ -1606,37 +1606,37 @@
         </is>
       </c>
       <c r="C28">
-        <v>19337900</v>
+        <v>32393616</v>
       </c>
       <c r="D28">
-        <v>387</v>
+        <v>433</v>
       </c>
       <c r="E28">
-        <v>49968.7338501292</v>
+        <v>74812.04618937644</v>
       </c>
       <c r="F28">
-        <v>1050493</v>
+        <v>1062305</v>
       </c>
       <c r="G28">
-        <v>18.4084044348701</v>
+        <v>30.49370566833443</v>
       </c>
       <c r="H28">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J28">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K28">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M28">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
@@ -1651,37 +1651,37 @@
         </is>
       </c>
       <c r="C29">
-        <v>15660506</v>
+        <v>37612520</v>
       </c>
       <c r="D29">
-        <v>814</v>
+        <v>1474</v>
       </c>
       <c r="E29">
-        <v>19238.95085995086</v>
+        <v>25517.31343283582</v>
       </c>
       <c r="F29">
-        <v>1920076</v>
+        <v>1929268</v>
       </c>
       <c r="G29">
-        <v>8.156190692451757</v>
+        <v>19.49574657331174</v>
       </c>
       <c r="H29">
         <v>42</v>
       </c>
       <c r="I29">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J29">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K29">
         <v>37</v>
       </c>
       <c r="L29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M29">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -1696,37 +1696,37 @@
         </is>
       </c>
       <c r="C30">
-        <v>15951518</v>
+        <v>52047419</v>
       </c>
       <c r="D30">
-        <v>2836</v>
+        <v>3728</v>
       </c>
       <c r="E30">
-        <v>5624.653737658674</v>
+        <v>13961.21754291846</v>
       </c>
       <c r="F30">
-        <v>2998039</v>
+        <v>3034392</v>
       </c>
       <c r="G30">
-        <v>5.320650598607957</v>
+        <v>17.15250336805528</v>
       </c>
       <c r="H30">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I30">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J30">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K30">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L30">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="M30">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -1741,37 +1741,37 @@
         </is>
       </c>
       <c r="C31">
-        <v>13838597</v>
+        <v>21437305</v>
       </c>
       <c r="D31">
-        <v>985</v>
+        <v>1390</v>
       </c>
       <c r="E31">
-        <v>14049.33705583756</v>
+        <v>15422.52158273381</v>
       </c>
       <c r="F31">
-        <v>1342795</v>
+        <v>1356458</v>
       </c>
       <c r="G31">
-        <v>10.30581510952901</v>
+        <v>15.80388408634842</v>
       </c>
       <c r="H31">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I31">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="J31">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K31">
         <v>41</v>
       </c>
       <c r="L31">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="M31">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1786,19 +1786,19 @@
         </is>
       </c>
       <c r="C32">
-        <v>55524423</v>
+        <v>122527778</v>
       </c>
       <c r="D32">
-        <v>61850</v>
+        <v>85464</v>
       </c>
       <c r="E32">
-        <v>897.7271301535974</v>
+        <v>1433.677080408125</v>
       </c>
       <c r="F32">
-        <v>9005644</v>
+        <v>8908520</v>
       </c>
       <c r="G32">
-        <v>6.16551387107907</v>
+        <v>13.75399931750729</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -1813,10 +1813,10 @@
         <v>11</v>
       </c>
       <c r="L32">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M32">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33">
@@ -1831,37 +1831,37 @@
         </is>
       </c>
       <c r="C33">
-        <v>31306643</v>
+        <v>63891493</v>
       </c>
       <c r="D33">
-        <v>1245</v>
+        <v>1845</v>
       </c>
       <c r="E33">
-        <v>25145.89799196787</v>
+        <v>34629.53550135501</v>
       </c>
       <c r="F33">
-        <v>2088070</v>
+        <v>2095428</v>
       </c>
       <c r="G33">
-        <v>14.99310032709632</v>
+        <v>30.49090352901651</v>
       </c>
       <c r="H33">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I33">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J33">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K33">
         <v>36</v>
       </c>
       <c r="L33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M33">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
@@ -1876,19 +1876,19 @@
         </is>
       </c>
       <c r="C34">
-        <v>152607845</v>
+        <v>326212072</v>
       </c>
       <c r="D34">
-        <v>190288</v>
+        <v>248431</v>
       </c>
       <c r="E34">
-        <v>801.9835459934416</v>
+        <v>1313.089236045421</v>
       </c>
       <c r="F34">
-        <v>19849399</v>
+        <v>19542209</v>
       </c>
       <c r="G34">
-        <v>7.688285423654389</v>
+        <v>16.69269180367481</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1903,10 +1903,10 @@
         <v>4</v>
       </c>
       <c r="L34">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="M34">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35">
@@ -1921,25 +1921,25 @@
         </is>
       </c>
       <c r="C35">
-        <v>60229488</v>
+        <v>182810137</v>
       </c>
       <c r="D35">
-        <v>4602</v>
+        <v>6801</v>
       </c>
       <c r="E35">
-        <v>13087.67666232073</v>
+        <v>26879.89075136009</v>
       </c>
       <c r="F35">
-        <v>10273419</v>
+        <v>10383620</v>
       </c>
       <c r="G35">
-        <v>5.862652735179982</v>
+        <v>17.60562665043598</v>
       </c>
       <c r="H35">
         <v>20</v>
       </c>
       <c r="I35">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J35">
         <v>3</v>
@@ -1948,10 +1948,10 @@
         <v>9</v>
       </c>
       <c r="L35">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="M35">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
@@ -1966,37 +1966,37 @@
         </is>
       </c>
       <c r="C36">
-        <v>9641944</v>
+        <v>18432100</v>
       </c>
       <c r="D36">
-        <v>308</v>
+        <v>585</v>
       </c>
       <c r="E36">
-        <v>31305.01298701299</v>
+        <v>31507.86324786325</v>
       </c>
       <c r="F36">
-        <v>755393</v>
+        <v>760077</v>
       </c>
       <c r="G36">
-        <v>12.76414263833528</v>
+        <v>24.25030621897518</v>
       </c>
       <c r="H36">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I36">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J36">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="K36">
         <v>47</v>
       </c>
       <c r="L36">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M36">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37">
@@ -2011,28 +2011,28 @@
         </is>
       </c>
       <c r="C37">
-        <v>76966291</v>
+        <v>198218013</v>
       </c>
       <c r="D37">
-        <v>6604</v>
+        <v>11602</v>
       </c>
       <c r="E37">
-        <v>11654.49591156875</v>
+        <v>17084.81408377866</v>
       </c>
       <c r="F37">
-        <v>11658609</v>
+        <v>11689442</v>
       </c>
       <c r="G37">
-        <v>6.601670147785212</v>
+        <v>16.95701240486928</v>
       </c>
       <c r="H37">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I37">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J37">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K37">
         <v>7</v>
@@ -2056,37 +2056,37 @@
         </is>
       </c>
       <c r="C38">
-        <v>35271126</v>
+        <v>129650876</v>
       </c>
       <c r="D38">
-        <v>1970</v>
+        <v>2599</v>
       </c>
       <c r="E38">
-        <v>17904.12487309645</v>
+        <v>49884.90804155445</v>
       </c>
       <c r="F38">
-        <v>3930864</v>
+        <v>3943079</v>
       </c>
       <c r="G38">
-        <v>8.972868560194399</v>
+        <v>32.88061842027512</v>
       </c>
       <c r="H38">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I38">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J38">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K38">
         <v>28</v>
       </c>
       <c r="L38">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M38">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
@@ -2101,37 +2101,37 @@
         </is>
       </c>
       <c r="C39">
-        <v>42445964</v>
+        <v>82919636</v>
       </c>
       <c r="D39">
-        <v>1527</v>
+        <v>1910</v>
       </c>
       <c r="E39">
-        <v>27796.96398166339</v>
+        <v>43413.4219895288</v>
       </c>
       <c r="F39">
-        <v>4142776</v>
+        <v>4190713</v>
       </c>
       <c r="G39">
-        <v>10.24577819317289</v>
+        <v>19.78652224573718</v>
       </c>
       <c r="H39">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J39">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K39">
         <v>27</v>
       </c>
       <c r="L39">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="M39">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -2146,37 +2146,37 @@
         </is>
       </c>
       <c r="C40">
-        <v>82353417</v>
+        <v>195196332</v>
       </c>
       <c r="D40">
-        <v>23036</v>
+        <v>32991</v>
       </c>
       <c r="E40">
-        <v>3574.987714881056</v>
+        <v>5916.653996544512</v>
       </c>
       <c r="F40">
-        <v>12805537</v>
+        <v>12807060</v>
       </c>
       <c r="G40">
-        <v>6.431078759133647</v>
+        <v>15.24130690416067</v>
       </c>
       <c r="H40">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I40">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K40">
         <v>5</v>
       </c>
       <c r="L40">
+        <v>47</v>
+      </c>
+      <c r="M40">
         <v>42</v>
-      </c>
-      <c r="M40">
-        <v>37</v>
       </c>
     </row>
     <row r="41">
@@ -2191,37 +2191,37 @@
         </is>
       </c>
       <c r="C41">
-        <v>15395742</v>
+        <v>24487613</v>
       </c>
       <c r="D41">
-        <v>2665</v>
+        <v>4706</v>
       </c>
       <c r="E41">
-        <v>5777.013883677299</v>
+        <v>5203.487675308117</v>
       </c>
       <c r="F41">
-        <v>1059639</v>
+        <v>1057315</v>
       </c>
       <c r="G41">
-        <v>14.52923306899803</v>
+        <v>23.1601868884864</v>
       </c>
       <c r="H41">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I41">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="J41">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="K41">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L41">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M41">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42">
@@ -2236,37 +2236,37 @@
         </is>
       </c>
       <c r="C42">
-        <v>36151921</v>
+        <v>102890537</v>
       </c>
       <c r="D42">
-        <v>3320</v>
+        <v>4382</v>
       </c>
       <c r="E42">
-        <v>10889.1328313253</v>
+        <v>23480.26859881333</v>
       </c>
       <c r="F42">
-        <v>5024369</v>
+        <v>5084127</v>
       </c>
       <c r="G42">
-        <v>7.195315670485189</v>
+        <v>20.23760165707898</v>
       </c>
       <c r="H42">
         <v>25</v>
       </c>
       <c r="I42">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K42">
         <v>23</v>
       </c>
       <c r="L42">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="M42">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2281,37 +2281,37 @@
         </is>
       </c>
       <c r="C43">
-        <v>10231886</v>
+        <v>26722632</v>
       </c>
       <c r="D43">
-        <v>730</v>
+        <v>1636</v>
       </c>
       <c r="E43">
-        <v>14016.28219178082</v>
+        <v>16334.1271393643</v>
       </c>
       <c r="F43">
-        <v>869666</v>
+        <v>882235</v>
       </c>
       <c r="G43">
-        <v>11.7653053011156</v>
+        <v>30.28969832300918</v>
       </c>
       <c r="H43">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I43">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J43">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="K43">
         <v>46</v>
       </c>
       <c r="L43">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M43">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44">
@@ -2326,37 +2326,37 @@
         </is>
       </c>
       <c r="C44">
-        <v>53160247</v>
+        <v>139727833</v>
       </c>
       <c r="D44">
-        <v>5508</v>
+        <v>7070</v>
       </c>
       <c r="E44">
-        <v>9651.460965867829</v>
+        <v>19763.48415841584</v>
       </c>
       <c r="F44">
-        <v>6715984</v>
+        <v>6770010</v>
       </c>
       <c r="G44">
-        <v>7.915481484172684</v>
+        <v>20.639235835693</v>
       </c>
       <c r="H44">
         <v>19</v>
       </c>
       <c r="I44">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J44">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K44">
         <v>16</v>
       </c>
       <c r="L44">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="M44">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -2371,37 +2371,37 @@
         </is>
       </c>
       <c r="C45">
-        <v>162768263</v>
+        <v>543994385</v>
       </c>
       <c r="D45">
-        <v>13886</v>
+        <v>19411</v>
       </c>
       <c r="E45">
-        <v>11721.75306063661</v>
+        <v>28025.05718407089</v>
       </c>
       <c r="F45">
-        <v>28304596</v>
+        <v>28701845</v>
       </c>
       <c r="G45">
-        <v>5.75059481506113</v>
+        <v>18.95328976238287</v>
       </c>
       <c r="H45">
         <v>10</v>
       </c>
       <c r="I45">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J45">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K45">
         <v>2</v>
       </c>
       <c r="L45">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="M45">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46">
@@ -2416,37 +2416,37 @@
         </is>
       </c>
       <c r="C46">
-        <v>20897088</v>
+        <v>63352248</v>
       </c>
       <c r="D46">
-        <v>2303</v>
+        <v>3069</v>
       </c>
       <c r="E46">
-        <v>9073.854971775945</v>
+        <v>20642.63538611926</v>
       </c>
       <c r="F46">
-        <v>3101833</v>
+        <v>3161105</v>
       </c>
       <c r="G46">
-        <v>6.737012598679555</v>
+        <v>20.04117167889077</v>
       </c>
       <c r="H46">
         <v>29</v>
       </c>
       <c r="I46">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K46">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L46">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="M46">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -2461,37 +2461,37 @@
         </is>
       </c>
       <c r="C47">
-        <v>15697419</v>
+        <v>20511243</v>
       </c>
       <c r="D47">
-        <v>748</v>
+        <v>816</v>
       </c>
       <c r="E47">
-        <v>20985.85427807487</v>
+        <v>25136.32720588235</v>
       </c>
       <c r="F47">
-        <v>623657</v>
+        <v>626299</v>
       </c>
       <c r="G47">
-        <v>25.16995560059456</v>
+        <v>32.74992136343823</v>
       </c>
       <c r="H47">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I47">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J47">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K47">
         <v>50</v>
       </c>
       <c r="L47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M47">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48">
@@ -2506,28 +2506,28 @@
         </is>
       </c>
       <c r="C48">
-        <v>43497577</v>
+        <v>117088286</v>
       </c>
       <c r="D48">
-        <v>5747</v>
+        <v>8669</v>
       </c>
       <c r="E48">
-        <v>7568.744910388029</v>
+        <v>13506.55046718191</v>
       </c>
       <c r="F48">
-        <v>8470020</v>
+        <v>8517685</v>
       </c>
       <c r="G48">
-        <v>5.135475122845047</v>
+        <v>13.74649168171868</v>
       </c>
       <c r="H48">
         <v>18</v>
       </c>
       <c r="I48">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J48">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K48">
         <v>12</v>
@@ -2551,25 +2551,25 @@
         </is>
       </c>
       <c r="C49">
-        <v>65424260</v>
+        <v>134329919</v>
       </c>
       <c r="D49">
-        <v>10609</v>
+        <v>12255</v>
       </c>
       <c r="E49">
-        <v>6166.863983410312</v>
+        <v>10961.2337005304</v>
       </c>
       <c r="F49">
-        <v>7405743</v>
+        <v>7535591</v>
       </c>
       <c r="G49">
-        <v>8.834260114076333</v>
+        <v>17.82606287947422</v>
       </c>
       <c r="H49">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I49">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J49">
         <v>24</v>
@@ -2578,10 +2578,10 @@
         <v>13</v>
       </c>
       <c r="L49">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="M49">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50">
@@ -2596,37 +2596,37 @@
         </is>
       </c>
       <c r="C50">
-        <v>30983620</v>
+        <v>54464892</v>
       </c>
       <c r="D50">
-        <v>611</v>
+        <v>890</v>
       </c>
       <c r="E50">
-        <v>50709.68903436988</v>
+        <v>61196.50786516854</v>
       </c>
       <c r="F50">
-        <v>1815857</v>
+        <v>1805832</v>
       </c>
       <c r="G50">
-        <v>17.0628083599094</v>
+        <v>30.16055314115599</v>
       </c>
       <c r="H50">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J50">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K50">
         <v>38</v>
       </c>
       <c r="L50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M50">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51">
@@ -2641,28 +2641,28 @@
         </is>
       </c>
       <c r="C51">
-        <v>35249718</v>
+        <v>90018423</v>
       </c>
       <c r="D51">
-        <v>3341</v>
+        <v>4347</v>
       </c>
       <c r="E51">
-        <v>10550.64890751272</v>
+        <v>20708.1718426501</v>
       </c>
       <c r="F51">
-        <v>5795483</v>
+        <v>5813568</v>
       </c>
       <c r="G51">
-        <v>6.082274419578144</v>
+        <v>15.48419542009313</v>
       </c>
       <c r="H51">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I51">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K51">
         <v>20</v>
@@ -2686,37 +2686,37 @@
         </is>
       </c>
       <c r="C52">
-        <v>10194407</v>
+        <v>15443610</v>
       </c>
       <c r="D52">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="E52">
-        <v>37757.06296296296</v>
+        <v>49340.60702875399</v>
       </c>
       <c r="F52">
-        <v>579315</v>
+        <v>577737</v>
       </c>
       <c r="G52">
-        <v>17.59734686655792</v>
+        <v>26.73121160666532</v>
       </c>
       <c r="H52">
         <v>51</v>
       </c>
       <c r="I52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J52">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K52">
         <v>51</v>
       </c>
       <c r="L52">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M52">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>